<commit_message>
nova base de dados
</commit_message>
<xml_diff>
--- a/tweets_normalizados_2020.xlsx
+++ b/tweets_normalizados_2020.xlsx
@@ -1804,7 +1804,7 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B106" t="n">
         <v>1.344350143982797e+18</v>
@@ -2129,7 +2129,7 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B131" t="n">
         <v>1.342977576046891e+18</v>
@@ -2160,10 +2160,8 @@
       <c r="B133" t="n">
         <v>1.342974502645494e+18</v>
       </c>
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>transfobia  e  suicidio</t>
-        </is>
+      <c r="C133" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="134">
@@ -2402,7 +2400,7 @@
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B152" t="n">
         <v>1.342972794653602e+18</v>
@@ -3623,7 +3621,9 @@
       </c>
     </row>
     <row r="246">
-      <c r="A246" t="inlineStr"/>
+      <c r="A246" t="n">
+        <v>1</v>
+      </c>
       <c r="B246" t="n">
         <v>1.342959266601325e+18</v>
       </c>
@@ -3634,7 +3634,9 @@
       </c>
     </row>
     <row r="247">
-      <c r="A247" t="inlineStr"/>
+      <c r="A247" t="n">
+        <v>2</v>
+      </c>
       <c r="B247" t="n">
         <v>1.342959041832743e+18</v>
       </c>
@@ -3645,7 +3647,9 @@
       </c>
     </row>
     <row r="248">
-      <c r="A248" t="inlineStr"/>
+      <c r="A248" t="n">
+        <v>3</v>
+      </c>
       <c r="B248" t="n">
         <v>1.342958942926889e+18</v>
       </c>
@@ -3656,7 +3660,9 @@
       </c>
     </row>
     <row r="249">
-      <c r="A249" t="inlineStr"/>
+      <c r="A249" t="n">
+        <v>3</v>
+      </c>
       <c r="B249" t="n">
         <v>1.34295861791864e+18</v>
       </c>
@@ -3667,7 +3673,9 @@
       </c>
     </row>
     <row r="250">
-      <c r="A250" t="inlineStr"/>
+      <c r="A250" t="n">
+        <v>1</v>
+      </c>
       <c r="B250" t="n">
         <v>1.34295861603534e+18</v>
       </c>
@@ -3678,7 +3686,9 @@
       </c>
     </row>
     <row r="251">
-      <c r="A251" t="inlineStr"/>
+      <c r="A251" t="n">
+        <v>1</v>
+      </c>
       <c r="B251" t="n">
         <v>1.342958564944585e+18</v>
       </c>
@@ -3702,7 +3712,9 @@
       </c>
     </row>
     <row r="253">
-      <c r="A253" t="inlineStr"/>
+      <c r="A253" t="n">
+        <v>1</v>
+      </c>
       <c r="B253" t="n">
         <v>1.342958205270426e+18</v>
       </c>
@@ -3713,7 +3725,9 @@
       </c>
     </row>
     <row r="254">
-      <c r="A254" t="inlineStr"/>
+      <c r="A254" t="n">
+        <v>1</v>
+      </c>
       <c r="B254" t="n">
         <v>1.3429580999347e+18</v>
       </c>
@@ -3724,7 +3738,9 @@
       </c>
     </row>
     <row r="255">
-      <c r="A255" t="inlineStr"/>
+      <c r="A255" t="n">
+        <v>2</v>
+      </c>
       <c r="B255" t="n">
         <v>1.342958068561285e+18</v>
       </c>
@@ -3735,7 +3751,9 @@
       </c>
     </row>
     <row r="256">
-      <c r="A256" t="inlineStr"/>
+      <c r="A256" t="n">
+        <v>1</v>
+      </c>
       <c r="B256" t="n">
         <v>1.342957664985342e+18</v>
       </c>
@@ -3746,7 +3764,9 @@
       </c>
     </row>
     <row r="257">
-      <c r="A257" t="inlineStr"/>
+      <c r="A257" t="n">
+        <v>3</v>
+      </c>
       <c r="B257" t="n">
         <v>1.34295749259527e+18</v>
       </c>
@@ -3757,7 +3777,9 @@
       </c>
     </row>
     <row r="258">
-      <c r="A258" t="inlineStr"/>
+      <c r="A258" t="n">
+        <v>3</v>
+      </c>
       <c r="B258" t="n">
         <v>1.342957456012542e+18</v>
       </c>
@@ -3781,7 +3803,9 @@
       </c>
     </row>
     <row r="260">
-      <c r="A260" t="inlineStr"/>
+      <c r="A260" t="n">
+        <v>3</v>
+      </c>
       <c r="B260" t="n">
         <v>1.342957325016048e+18</v>
       </c>
@@ -3792,7 +3816,9 @@
       </c>
     </row>
     <row r="261">
-      <c r="A261" t="inlineStr"/>
+      <c r="A261" t="n">
+        <v>3</v>
+      </c>
       <c r="B261" t="n">
         <v>1.342957248067359e+18</v>
       </c>
@@ -3803,7 +3829,9 @@
       </c>
     </row>
     <row r="262">
-      <c r="A262" t="inlineStr"/>
+      <c r="A262" t="n">
+        <v>3</v>
+      </c>
       <c r="B262" t="n">
         <v>1.342957240257548e+18</v>
       </c>
@@ -3814,7 +3842,9 @@
       </c>
     </row>
     <row r="263">
-      <c r="A263" t="inlineStr"/>
+      <c r="A263" t="n">
+        <v>1</v>
+      </c>
       <c r="B263" t="n">
         <v>1.342957166685254e+18</v>
       </c>
@@ -3825,7 +3855,9 @@
       </c>
     </row>
     <row r="264">
-      <c r="A264" t="inlineStr"/>
+      <c r="A264" t="n">
+        <v>3</v>
+      </c>
       <c r="B264" t="n">
         <v>1.342956977492812e+18</v>
       </c>
@@ -3836,7 +3868,9 @@
       </c>
     </row>
     <row r="265">
-      <c r="A265" t="inlineStr"/>
+      <c r="A265" t="n">
+        <v>1</v>
+      </c>
       <c r="B265" t="n">
         <v>1.342956748332806e+18</v>
       </c>
@@ -3847,7 +3881,9 @@
       </c>
     </row>
     <row r="266">
-      <c r="A266" t="inlineStr"/>
+      <c r="A266" t="n">
+        <v>3</v>
+      </c>
       <c r="B266" t="n">
         <v>1.342956715143266e+18</v>
       </c>
@@ -3858,7 +3894,9 @@
       </c>
     </row>
     <row r="267">
-      <c r="A267" t="inlineStr"/>
+      <c r="A267" t="n">
+        <v>3</v>
+      </c>
       <c r="B267" t="n">
         <v>1.342955808028557e+18</v>
       </c>
@@ -3869,7 +3907,9 @@
       </c>
     </row>
     <row r="268">
-      <c r="A268" t="inlineStr"/>
+      <c r="A268" t="n">
+        <v>1</v>
+      </c>
       <c r="B268" t="n">
         <v>1.342955690739032e+18</v>
       </c>
@@ -3880,7 +3920,9 @@
       </c>
     </row>
     <row r="269">
-      <c r="A269" t="inlineStr"/>
+      <c r="A269" t="n">
+        <v>2</v>
+      </c>
       <c r="B269" t="n">
         <v>1.342955645985812e+18</v>
       </c>
@@ -3891,7 +3933,9 @@
       </c>
     </row>
     <row r="270">
-      <c r="A270" t="inlineStr"/>
+      <c r="A270" t="n">
+        <v>1</v>
+      </c>
       <c r="B270" t="n">
         <v>1.34295553670323e+18</v>
       </c>
@@ -3902,7 +3946,9 @@
       </c>
     </row>
     <row r="271">
-      <c r="A271" t="inlineStr"/>
+      <c r="A271" t="n">
+        <v>1</v>
+      </c>
       <c r="B271" t="n">
         <v>1.342955294654165e+18</v>
       </c>
@@ -3913,7 +3959,9 @@
       </c>
     </row>
     <row r="272">
-      <c r="A272" t="inlineStr"/>
+      <c r="A272" t="n">
+        <v>3</v>
+      </c>
       <c r="B272" t="n">
         <v>1.342955265314927e+18</v>
       </c>
@@ -3924,7 +3972,9 @@
       </c>
     </row>
     <row r="273">
-      <c r="A273" t="inlineStr"/>
+      <c r="A273" t="n">
+        <v>1</v>
+      </c>
       <c r="B273" t="n">
         <v>1.34295521151044e+18</v>
       </c>
@@ -3948,7 +3998,9 @@
       </c>
     </row>
     <row r="275">
-      <c r="A275" t="inlineStr"/>
+      <c r="A275" t="n">
+        <v>1</v>
+      </c>
       <c r="B275" t="n">
         <v>1.342954785570517e+18</v>
       </c>
@@ -3959,7 +4011,9 @@
       </c>
     </row>
     <row r="276">
-      <c r="A276" t="inlineStr"/>
+      <c r="A276" t="n">
+        <v>3</v>
+      </c>
       <c r="B276" t="n">
         <v>1.34295475625225e+18</v>
       </c>
@@ -3970,7 +4024,9 @@
       </c>
     </row>
     <row r="277">
-      <c r="A277" t="inlineStr"/>
+      <c r="A277" t="n">
+        <v>1</v>
+      </c>
       <c r="B277" t="n">
         <v>1.342954672127156e+18</v>
       </c>
@@ -3981,7 +4037,9 @@
       </c>
     </row>
     <row r="278">
-      <c r="A278" t="inlineStr"/>
+      <c r="A278" t="n">
+        <v>1</v>
+      </c>
       <c r="B278" t="n">
         <v>1.342990265485767e+18</v>
       </c>
@@ -3992,7 +4050,9 @@
       </c>
     </row>
     <row r="279">
-      <c r="A279" t="inlineStr"/>
+      <c r="A279" t="n">
+        <v>3</v>
+      </c>
       <c r="B279" t="n">
         <v>1.342954387996619e+18</v>
       </c>
@@ -4016,7 +4076,9 @@
       </c>
     </row>
     <row r="281">
-      <c r="A281" t="inlineStr"/>
+      <c r="A281" t="n">
+        <v>3</v>
+      </c>
       <c r="B281" t="n">
         <v>1.342953784876683e+18</v>
       </c>
@@ -4027,7 +4089,9 @@
       </c>
     </row>
     <row r="282">
-      <c r="A282" t="inlineStr"/>
+      <c r="A282" t="n">
+        <v>3</v>
+      </c>
       <c r="B282" t="n">
         <v>1.34295361686118e+18</v>
       </c>
@@ -4038,7 +4102,9 @@
       </c>
     </row>
     <row r="283">
-      <c r="A283" t="inlineStr"/>
+      <c r="A283" t="n">
+        <v>3</v>
+      </c>
       <c r="B283" t="n">
         <v>1.342953425454191e+18</v>
       </c>
@@ -4062,7 +4128,9 @@
       </c>
     </row>
     <row r="285">
-      <c r="A285" t="inlineStr"/>
+      <c r="A285" t="n">
+        <v>2</v>
+      </c>
       <c r="B285" t="n">
         <v>1.34295332158643e+18</v>
       </c>
@@ -4073,7 +4141,9 @@
       </c>
     </row>
     <row r="286">
-      <c r="A286" t="inlineStr"/>
+      <c r="A286" t="n">
+        <v>3</v>
+      </c>
       <c r="B286" t="n">
         <v>1.342953174332797e+18</v>
       </c>
@@ -4084,7 +4154,9 @@
       </c>
     </row>
     <row r="287">
-      <c r="A287" t="inlineStr"/>
+      <c r="A287" t="n">
+        <v>1</v>
+      </c>
       <c r="B287" t="n">
         <v>1.342953168599179e+18</v>
       </c>
@@ -4095,7 +4167,9 @@
       </c>
     </row>
     <row r="288">
-      <c r="A288" t="inlineStr"/>
+      <c r="A288" t="n">
+        <v>2</v>
+      </c>
       <c r="B288" t="n">
         <v>1.34295305251765e+18</v>
       </c>
@@ -4106,7 +4180,9 @@
       </c>
     </row>
     <row r="289">
-      <c r="A289" t="inlineStr"/>
+      <c r="A289" t="n">
+        <v>1</v>
+      </c>
       <c r="B289" t="n">
         <v>1.342952949467783e+18</v>
       </c>
@@ -4117,7 +4193,9 @@
       </c>
     </row>
     <row r="290">
-      <c r="A290" t="inlineStr"/>
+      <c r="A290" t="n">
+        <v>1</v>
+      </c>
       <c r="B290" t="n">
         <v>1.342952596852638e+18</v>
       </c>
@@ -4128,7 +4206,9 @@
       </c>
     </row>
     <row r="291">
-      <c r="A291" t="inlineStr"/>
+      <c r="A291" t="n">
+        <v>2</v>
+      </c>
       <c r="B291" t="n">
         <v>1.342979280507171e+18</v>
       </c>
@@ -4139,7 +4219,9 @@
       </c>
     </row>
     <row r="292">
-      <c r="A292" t="inlineStr"/>
+      <c r="A292" t="n">
+        <v>3</v>
+      </c>
       <c r="B292" t="n">
         <v>1.342952202290287e+18</v>
       </c>
@@ -4150,7 +4232,9 @@
       </c>
     </row>
     <row r="293">
-      <c r="A293" t="inlineStr"/>
+      <c r="A293" t="n">
+        <v>3</v>
+      </c>
       <c r="B293" t="n">
         <v>1.34295219878382e+18</v>
       </c>
@@ -4161,7 +4245,9 @@
       </c>
     </row>
     <row r="294">
-      <c r="A294" t="inlineStr"/>
+      <c r="A294" t="n">
+        <v>3</v>
+      </c>
       <c r="B294" t="n">
         <v>1.342952029598216e+18</v>
       </c>
@@ -4172,7 +4258,9 @@
       </c>
     </row>
     <row r="295">
-      <c r="A295" t="inlineStr"/>
+      <c r="A295" t="n">
+        <v>1</v>
+      </c>
       <c r="B295" t="n">
         <v>1.342951955887518e+18</v>
       </c>
@@ -4183,7 +4271,9 @@
       </c>
     </row>
     <row r="296">
-      <c r="A296" t="inlineStr"/>
+      <c r="A296" t="n">
+        <v>2</v>
+      </c>
       <c r="B296" t="n">
         <v>1.342951666161754e+18</v>
       </c>
@@ -4194,7 +4284,9 @@
       </c>
     </row>
     <row r="297">
-      <c r="A297" t="inlineStr"/>
+      <c r="A297" t="n">
+        <v>3</v>
+      </c>
       <c r="B297" t="n">
         <v>1.342951423747752e+18</v>
       </c>
@@ -4205,7 +4297,9 @@
       </c>
     </row>
     <row r="298">
-      <c r="A298" t="inlineStr"/>
+      <c r="A298" t="n">
+        <v>3</v>
+      </c>
       <c r="B298" t="n">
         <v>1.34295108154708e+18</v>
       </c>
@@ -4216,7 +4310,9 @@
       </c>
     </row>
     <row r="299">
-      <c r="A299" t="inlineStr"/>
+      <c r="A299" t="n">
+        <v>3</v>
+      </c>
       <c r="B299" t="n">
         <v>1.342951019018334e+18</v>
       </c>
@@ -4227,7 +4323,9 @@
       </c>
     </row>
     <row r="300">
-      <c r="A300" t="inlineStr"/>
+      <c r="A300" t="n">
+        <v>3</v>
+      </c>
       <c r="B300" t="n">
         <v>1.342950942870798e+18</v>
       </c>
@@ -4238,7 +4336,9 @@
       </c>
     </row>
     <row r="301">
-      <c r="A301" t="inlineStr"/>
+      <c r="A301" t="n">
+        <v>1</v>
+      </c>
       <c r="B301" t="n">
         <v>1.342950752130576e+18</v>
       </c>
@@ -4249,7 +4349,9 @@
       </c>
     </row>
     <row r="302">
-      <c r="A302" t="inlineStr"/>
+      <c r="A302" t="n">
+        <v>2</v>
+      </c>
       <c r="B302" t="n">
         <v>1.342950735001084e+18</v>
       </c>
@@ -4260,7 +4362,9 @@
       </c>
     </row>
     <row r="303">
-      <c r="A303" t="inlineStr"/>
+      <c r="A303" t="n">
+        <v>2</v>
+      </c>
       <c r="B303" t="n">
         <v>1.342950695100682e+18</v>
       </c>
@@ -4271,7 +4375,9 @@
       </c>
     </row>
     <row r="304">
-      <c r="A304" t="inlineStr"/>
+      <c r="A304" t="n">
+        <v>2</v>
+      </c>
       <c r="B304" t="n">
         <v>1.343001505029386e+18</v>
       </c>
@@ -4282,7 +4388,9 @@
       </c>
     </row>
     <row r="305">
-      <c r="A305" t="inlineStr"/>
+      <c r="A305" t="n">
+        <v>2</v>
+      </c>
       <c r="B305" t="n">
         <v>1.342950449993961e+18</v>
       </c>
@@ -4293,7 +4401,9 @@
       </c>
     </row>
     <row r="306">
-      <c r="A306" t="inlineStr"/>
+      <c r="A306" t="n">
+        <v>3</v>
+      </c>
       <c r="B306" t="n">
         <v>1.342950430230381e+18</v>
       </c>
@@ -4304,7 +4414,9 @@
       </c>
     </row>
     <row r="307">
-      <c r="A307" t="inlineStr"/>
+      <c r="A307" t="n">
+        <v>2</v>
+      </c>
       <c r="B307" t="n">
         <v>1.342950089678008e+18</v>
       </c>
@@ -4315,7 +4427,9 @@
       </c>
     </row>
     <row r="308">
-      <c r="A308" t="inlineStr"/>
+      <c r="A308" t="n">
+        <v>3</v>
+      </c>
       <c r="B308" t="n">
         <v>1.342949964004135e+18</v>
       </c>
@@ -4339,7 +4453,9 @@
       </c>
     </row>
     <row r="310">
-      <c r="A310" t="inlineStr"/>
+      <c r="A310" t="n">
+        <v>2</v>
+      </c>
       <c r="B310" t="n">
         <v>1.342949604271256e+18</v>
       </c>
@@ -4350,7 +4466,9 @@
       </c>
     </row>
     <row r="311">
-      <c r="A311" t="inlineStr"/>
+      <c r="A311" t="n">
+        <v>2</v>
+      </c>
       <c r="B311" t="n">
         <v>1.342949558339445e+18</v>
       </c>
@@ -4361,7 +4479,9 @@
       </c>
     </row>
     <row r="312">
-      <c r="A312" t="inlineStr"/>
+      <c r="A312" t="n">
+        <v>3</v>
+      </c>
       <c r="B312" t="n">
         <v>1.342949219452269e+18</v>
       </c>
@@ -4372,7 +4492,9 @@
       </c>
     </row>
     <row r="313">
-      <c r="A313" t="inlineStr"/>
+      <c r="A313" t="n">
+        <v>2</v>
+      </c>
       <c r="B313" t="n">
         <v>1.342948947816575e+18</v>
       </c>
@@ -4383,7 +4505,9 @@
       </c>
     </row>
     <row r="314">
-      <c r="A314" t="inlineStr"/>
+      <c r="A314" t="n">
+        <v>3</v>
+      </c>
       <c r="B314" t="n">
         <v>1.342948740336939e+18</v>
       </c>
@@ -4394,7 +4518,9 @@
       </c>
     </row>
     <row r="315">
-      <c r="A315" t="inlineStr"/>
+      <c r="A315" t="n">
+        <v>2</v>
+      </c>
       <c r="B315" t="n">
         <v>1.342948618811138e+18</v>
       </c>
@@ -4418,7 +4544,9 @@
       </c>
     </row>
     <row r="317">
-      <c r="A317" t="inlineStr"/>
+      <c r="A317" t="n">
+        <v>3</v>
+      </c>
       <c r="B317" t="n">
         <v>1.342948161845866e+18</v>
       </c>
@@ -4429,7 +4557,9 @@
       </c>
     </row>
     <row r="318">
-      <c r="A318" t="inlineStr"/>
+      <c r="A318" t="n">
+        <v>1</v>
+      </c>
       <c r="B318" t="n">
         <v>1.342948128568308e+18</v>
       </c>
@@ -4440,7 +4570,9 @@
       </c>
     </row>
     <row r="319">
-      <c r="A319" t="inlineStr"/>
+      <c r="A319" t="n">
+        <v>2</v>
+      </c>
       <c r="B319" t="n">
         <v>1.342947695594496e+18</v>
       </c>
@@ -4451,7 +4583,9 @@
       </c>
     </row>
     <row r="320">
-      <c r="A320" t="inlineStr"/>
+      <c r="A320" t="n">
+        <v>3</v>
+      </c>
       <c r="B320" t="n">
         <v>1.342947125043352e+18</v>
       </c>
@@ -4462,7 +4596,9 @@
       </c>
     </row>
     <row r="321">
-      <c r="A321" t="inlineStr"/>
+      <c r="A321" t="n">
+        <v>1</v>
+      </c>
       <c r="B321" t="n">
         <v>1.342947076079038e+18</v>
       </c>
@@ -4473,7 +4609,9 @@
       </c>
     </row>
     <row r="322">
-      <c r="A322" t="inlineStr"/>
+      <c r="A322" t="n">
+        <v>2</v>
+      </c>
       <c r="B322" t="n">
         <v>1.342946996240396e+18</v>
       </c>
@@ -4497,7 +4635,9 @@
       </c>
     </row>
     <row r="324">
-      <c r="A324" t="inlineStr"/>
+      <c r="A324" t="n">
+        <v>3</v>
+      </c>
       <c r="B324" t="n">
         <v>1.342946889285693e+18</v>
       </c>
@@ -4508,7 +4648,9 @@
       </c>
     </row>
     <row r="325">
-      <c r="A325" t="inlineStr"/>
+      <c r="A325" t="n">
+        <v>3</v>
+      </c>
       <c r="B325" t="n">
         <v>1.34294613288074e+18</v>
       </c>
@@ -4545,7 +4687,9 @@
       </c>
     </row>
     <row r="328">
-      <c r="A328" t="inlineStr"/>
+      <c r="A328" t="n">
+        <v>1</v>
+      </c>
       <c r="B328" t="n">
         <v>1.342945968539525e+18</v>
       </c>
@@ -4556,7 +4700,9 @@
       </c>
     </row>
     <row r="329">
-      <c r="A329" t="inlineStr"/>
+      <c r="A329" t="n">
+        <v>1</v>
+      </c>
       <c r="B329" t="n">
         <v>1.342945966937305e+18</v>
       </c>
@@ -4567,7 +4713,9 @@
       </c>
     </row>
     <row r="330">
-      <c r="A330" t="inlineStr"/>
+      <c r="A330" t="n">
+        <v>1</v>
+      </c>
       <c r="B330" t="n">
         <v>1.342945832048472e+18</v>
       </c>
@@ -4578,7 +4726,9 @@
       </c>
     </row>
     <row r="331">
-      <c r="A331" t="inlineStr"/>
+      <c r="A331" t="n">
+        <v>1</v>
+      </c>
       <c r="B331" t="n">
         <v>1.342945397669569e+18</v>
       </c>
@@ -4589,7 +4739,9 @@
       </c>
     </row>
     <row r="332">
-      <c r="A332" t="inlineStr"/>
+      <c r="A332" t="n">
+        <v>3</v>
+      </c>
       <c r="B332" t="n">
         <v>1.342945386990809e+18</v>
       </c>
@@ -4600,7 +4752,9 @@
       </c>
     </row>
     <row r="333">
-      <c r="A333" t="inlineStr"/>
+      <c r="A333" t="n">
+        <v>2</v>
+      </c>
       <c r="B333" t="n">
         <v>1.342945143620514e+18</v>
       </c>
@@ -4637,7 +4791,9 @@
       </c>
     </row>
     <row r="336">
-      <c r="A336" t="inlineStr"/>
+      <c r="A336" t="n">
+        <v>3</v>
+      </c>
       <c r="B336" t="n">
         <v>1.342944563158245e+18</v>
       </c>
@@ -4648,7 +4804,9 @@
       </c>
     </row>
     <row r="337">
-      <c r="A337" t="inlineStr"/>
+      <c r="A337" t="n">
+        <v>1</v>
+      </c>
       <c r="B337" t="n">
         <v>1.3429444733959e+18</v>
       </c>
@@ -4672,7 +4830,9 @@
       </c>
     </row>
     <row r="339">
-      <c r="A339" t="inlineStr"/>
+      <c r="A339" t="n">
+        <v>1</v>
+      </c>
       <c r="B339" t="n">
         <v>1.342944421340467e+18</v>
       </c>
@@ -4683,7 +4843,9 @@
       </c>
     </row>
     <row r="340">
-      <c r="A340" t="inlineStr"/>
+      <c r="A340" t="n">
+        <v>3</v>
+      </c>
       <c r="B340" t="n">
         <v>1.342944274548204e+18</v>
       </c>
@@ -4694,7 +4856,9 @@
       </c>
     </row>
     <row r="341">
-      <c r="A341" t="inlineStr"/>
+      <c r="A341" t="n">
+        <v>2</v>
+      </c>
       <c r="B341" t="n">
         <v>1.342944153014051e+18</v>
       </c>
@@ -4705,7 +4869,9 @@
       </c>
     </row>
     <row r="342">
-      <c r="A342" t="inlineStr"/>
+      <c r="A342" t="n">
+        <v>2</v>
+      </c>
       <c r="B342" t="n">
         <v>1.342944029290459e+18</v>
       </c>
@@ -4742,7 +4908,9 @@
       </c>
     </row>
     <row r="345">
-      <c r="A345" t="inlineStr"/>
+      <c r="A345" t="n">
+        <v>1</v>
+      </c>
       <c r="B345" t="n">
         <v>1.342943867931402e+18</v>
       </c>
@@ -4753,7 +4921,9 @@
       </c>
     </row>
     <row r="346">
-      <c r="A346" t="inlineStr"/>
+      <c r="A346" t="n">
+        <v>3</v>
+      </c>
       <c r="B346" t="n">
         <v>1.342943557225763e+18</v>
       </c>
@@ -4764,7 +4934,9 @@
       </c>
     </row>
     <row r="347">
-      <c r="A347" t="inlineStr"/>
+      <c r="A347" t="n">
+        <v>2</v>
+      </c>
       <c r="B347" t="n">
         <v>1.342943427420369e+18</v>
       </c>
@@ -4775,7 +4947,9 @@
       </c>
     </row>
     <row r="348">
-      <c r="A348" t="inlineStr"/>
+      <c r="A348" t="n">
+        <v>2</v>
+      </c>
       <c r="B348" t="n">
         <v>1.342943271820124e+18</v>
       </c>
@@ -4786,7 +4960,9 @@
       </c>
     </row>
     <row r="349">
-      <c r="A349" t="inlineStr"/>
+      <c r="A349" t="n">
+        <v>2</v>
+      </c>
       <c r="B349" t="n">
         <v>1.342942979745571e+18</v>
       </c>
@@ -4797,7 +4973,9 @@
       </c>
     </row>
     <row r="350">
-      <c r="A350" t="inlineStr"/>
+      <c r="A350" t="n">
+        <v>1</v>
+      </c>
       <c r="B350" t="n">
         <v>1.342942876611863e+18</v>
       </c>
@@ -4821,7 +4999,9 @@
       </c>
     </row>
     <row r="352">
-      <c r="A352" t="inlineStr"/>
+      <c r="A352" t="n">
+        <v>1</v>
+      </c>
       <c r="B352" t="n">
         <v>1.342942376952787e+18</v>
       </c>
@@ -4832,7 +5012,9 @@
       </c>
     </row>
     <row r="353">
-      <c r="A353" t="inlineStr"/>
+      <c r="A353" t="n">
+        <v>2</v>
+      </c>
       <c r="B353" t="n">
         <v>1.342990613516575e+18</v>
       </c>
@@ -4843,7 +5025,9 @@
       </c>
     </row>
     <row r="354">
-      <c r="A354" t="inlineStr"/>
+      <c r="A354" t="n">
+        <v>3</v>
+      </c>
       <c r="B354" t="n">
         <v>1.342942096999723e+18</v>
       </c>
@@ -4854,7 +5038,9 @@
       </c>
     </row>
     <row r="355">
-      <c r="A355" t="inlineStr"/>
+      <c r="A355" t="n">
+        <v>1</v>
+      </c>
       <c r="B355" t="n">
         <v>1.342942044596138e+18</v>
       </c>
@@ -4865,7 +5051,9 @@
       </c>
     </row>
     <row r="356">
-      <c r="A356" t="inlineStr"/>
+      <c r="A356" t="n">
+        <v>1</v>
+      </c>
       <c r="B356" t="n">
         <v>1.342941959804117e+18</v>
       </c>
@@ -4876,7 +5064,9 @@
       </c>
     </row>
     <row r="357">
-      <c r="A357" t="inlineStr"/>
+      <c r="A357" t="n">
+        <v>1</v>
+      </c>
       <c r="B357" t="n">
         <v>1.34294184524508e+18</v>
       </c>
@@ -4887,7 +5077,9 @@
       </c>
     </row>
     <row r="358">
-      <c r="A358" t="inlineStr"/>
+      <c r="A358" t="n">
+        <v>1</v>
+      </c>
       <c r="B358" t="n">
         <v>1.342941833844945e+18</v>
       </c>
@@ -4898,7 +5090,9 @@
       </c>
     </row>
     <row r="359">
-      <c r="A359" t="inlineStr"/>
+      <c r="A359" t="n">
+        <v>3</v>
+      </c>
       <c r="B359" t="n">
         <v>1.342941656270725e+18</v>
       </c>
@@ -4909,7 +5103,9 @@
       </c>
     </row>
     <row r="360">
-      <c r="A360" t="inlineStr"/>
+      <c r="A360" t="n">
+        <v>3</v>
+      </c>
       <c r="B360" t="n">
         <v>1.342941184768029e+18</v>
       </c>
@@ -4920,7 +5116,9 @@
       </c>
     </row>
     <row r="361">
-      <c r="A361" t="inlineStr"/>
+      <c r="A361" t="n">
+        <v>3</v>
+      </c>
       <c r="B361" t="n">
         <v>1.342940984368361e+18</v>
       </c>
@@ -4931,7 +5129,9 @@
       </c>
     </row>
     <row r="362">
-      <c r="A362" t="inlineStr"/>
+      <c r="A362" t="n">
+        <v>2</v>
+      </c>
       <c r="B362" t="n">
         <v>1.343008486565798e+18</v>
       </c>
@@ -4942,7 +5142,9 @@
       </c>
     </row>
     <row r="363">
-      <c r="A363" t="inlineStr"/>
+      <c r="A363" t="n">
+        <v>1</v>
+      </c>
       <c r="B363" t="n">
         <v>1.342940382770946e+18</v>
       </c>
@@ -4953,7 +5155,9 @@
       </c>
     </row>
     <row r="364">
-      <c r="A364" t="inlineStr"/>
+      <c r="A364" t="n">
+        <v>3</v>
+      </c>
       <c r="B364" t="n">
         <v>1.34294023943895e+18</v>
       </c>
@@ -4964,7 +5168,9 @@
       </c>
     </row>
     <row r="365">
-      <c r="A365" t="inlineStr"/>
+      <c r="A365" t="n">
+        <v>1</v>
+      </c>
       <c r="B365" t="n">
         <v>1.3429402004236e+18</v>
       </c>
@@ -4975,7 +5181,9 @@
       </c>
     </row>
     <row r="366">
-      <c r="A366" t="inlineStr"/>
+      <c r="A366" t="n">
+        <v>1</v>
+      </c>
       <c r="B366" t="n">
         <v>1.342940153304723e+18</v>
       </c>
@@ -4986,7 +5194,9 @@
       </c>
     </row>
     <row r="367">
-      <c r="A367" t="inlineStr"/>
+      <c r="A367" t="n">
+        <v>2</v>
+      </c>
       <c r="B367" t="n">
         <v>1.342940120115241e+18</v>
       </c>
@@ -5010,7 +5220,9 @@
       </c>
     </row>
     <row r="369">
-      <c r="A369" t="inlineStr"/>
+      <c r="A369" t="n">
+        <v>1</v>
+      </c>
       <c r="B369" t="n">
         <v>1.342939195191554e+18</v>
       </c>
@@ -5021,7 +5233,9 @@
       </c>
     </row>
     <row r="370">
-      <c r="A370" t="inlineStr"/>
+      <c r="A370" t="n">
+        <v>3</v>
+      </c>
       <c r="B370" t="n">
         <v>1.342980086488834e+18</v>
       </c>
@@ -5032,7 +5246,9 @@
       </c>
     </row>
     <row r="371">
-      <c r="A371" t="inlineStr"/>
+      <c r="A371" t="n">
+        <v>1</v>
+      </c>
       <c r="B371" t="n">
         <v>1.342938989624513e+18</v>
       </c>
@@ -5043,7 +5259,9 @@
       </c>
     </row>
     <row r="372">
-      <c r="A372" t="inlineStr"/>
+      <c r="A372" t="n">
+        <v>3</v>
+      </c>
       <c r="B372" t="n">
         <v>1.342938860356067e+18</v>
       </c>
@@ -5054,7 +5272,9 @@
       </c>
     </row>
     <row r="373">
-      <c r="A373" t="inlineStr"/>
+      <c r="A373" t="n">
+        <v>1</v>
+      </c>
       <c r="B373" t="n">
         <v>1.342937402940273e+18</v>
       </c>
@@ -5065,7 +5285,9 @@
       </c>
     </row>
     <row r="374">
-      <c r="A374" t="inlineStr"/>
+      <c r="A374" t="n">
+        <v>3</v>
+      </c>
       <c r="B374" t="n">
         <v>1.342938837237064e+18</v>
       </c>
@@ -5076,7 +5298,9 @@
       </c>
     </row>
     <row r="375">
-      <c r="A375" t="inlineStr"/>
+      <c r="A375" t="n">
+        <v>1</v>
+      </c>
       <c r="B375" t="n">
         <v>1.342938627400225e+18</v>
       </c>
@@ -5087,7 +5311,9 @@
       </c>
     </row>
     <row r="376">
-      <c r="A376" t="inlineStr"/>
+      <c r="A376" t="n">
+        <v>1</v>
+      </c>
       <c r="B376" t="n">
         <v>1.342938609196945e+18</v>
       </c>
@@ -5111,7 +5337,9 @@
       </c>
     </row>
     <row r="378">
-      <c r="A378" t="inlineStr"/>
+      <c r="A378" t="n">
+        <v>1</v>
+      </c>
       <c r="B378" t="n">
         <v>1.342938387058192e+18</v>
       </c>
@@ -5122,7 +5350,9 @@
       </c>
     </row>
     <row r="379">
-      <c r="A379" t="inlineStr"/>
+      <c r="A379" t="n">
+        <v>3</v>
+      </c>
       <c r="B379" t="n">
         <v>1.342938354917249e+18</v>
       </c>
@@ -5146,7 +5376,9 @@
       </c>
     </row>
     <row r="381">
-      <c r="A381" t="inlineStr"/>
+      <c r="A381" t="n">
+        <v>1</v>
+      </c>
       <c r="B381" t="n">
         <v>1.342937903098429e+18</v>
       </c>
@@ -5170,7 +5402,9 @@
       </c>
     </row>
     <row r="383">
-      <c r="A383" t="inlineStr"/>
+      <c r="A383" t="n">
+        <v>1</v>
+      </c>
       <c r="B383" t="n">
         <v>1.342593671955427e+18</v>
       </c>
@@ -5194,7 +5428,9 @@
       </c>
     </row>
     <row r="385">
-      <c r="A385" t="inlineStr"/>
+      <c r="A385" t="n">
+        <v>3</v>
+      </c>
       <c r="B385" t="n">
         <v>1.34293738126832e+18</v>
       </c>
@@ -5205,7 +5441,9 @@
       </c>
     </row>
     <row r="386">
-      <c r="A386" t="inlineStr"/>
+      <c r="A386" t="n">
+        <v>2</v>
+      </c>
       <c r="B386" t="n">
         <v>1.342937331196682e+18</v>
       </c>
@@ -5216,7 +5454,9 @@
       </c>
     </row>
     <row r="387">
-      <c r="A387" t="inlineStr"/>
+      <c r="A387" t="n">
+        <v>3</v>
+      </c>
       <c r="B387" t="n">
         <v>1.342937084919755e+18</v>
       </c>
@@ -5227,7 +5467,9 @@
       </c>
     </row>
     <row r="388">
-      <c r="A388" t="inlineStr"/>
+      <c r="A388" t="n">
+        <v>3</v>
+      </c>
       <c r="B388" t="n">
         <v>1.342937067454685e+18</v>
       </c>
@@ -5251,7 +5493,9 @@
       </c>
     </row>
     <row r="390">
-      <c r="A390" t="inlineStr"/>
+      <c r="A390" t="n">
+        <v>3</v>
+      </c>
       <c r="B390" t="n">
         <v>1.342936091884708e+18</v>
       </c>
@@ -5262,7 +5506,9 @@
       </c>
     </row>
     <row r="391">
-      <c r="A391" t="inlineStr"/>
+      <c r="A391" t="n">
+        <v>2</v>
+      </c>
       <c r="B391" t="n">
         <v>1.342935763919524e+18</v>
       </c>
@@ -5273,7 +5519,9 @@
       </c>
     </row>
     <row r="392">
-      <c r="A392" t="inlineStr"/>
+      <c r="A392" t="n">
+        <v>1</v>
+      </c>
       <c r="B392" t="n">
         <v>1.342935631241085e+18</v>
       </c>
@@ -5310,7 +5558,9 @@
       </c>
     </row>
     <row r="395">
-      <c r="A395" t="inlineStr"/>
+      <c r="A395" t="n">
+        <v>1</v>
+      </c>
       <c r="B395" t="n">
         <v>1.342935340122825e+18</v>
       </c>
@@ -5321,7 +5571,9 @@
       </c>
     </row>
     <row r="396">
-      <c r="A396" t="inlineStr"/>
+      <c r="A396" t="n">
+        <v>1</v>
+      </c>
       <c r="B396" t="n">
         <v>1.342935295231189e+18</v>
       </c>
@@ -5332,7 +5584,9 @@
       </c>
     </row>
     <row r="397">
-      <c r="A397" t="inlineStr"/>
+      <c r="A397" t="n">
+        <v>3</v>
+      </c>
       <c r="B397" t="n">
         <v>1.342935190939775e+18</v>
       </c>
@@ -5343,7 +5597,9 @@
       </c>
     </row>
     <row r="398">
-      <c r="A398" t="inlineStr"/>
+      <c r="A398" t="n">
+        <v>1</v>
+      </c>
       <c r="B398" t="n">
         <v>1.342935170270327e+18</v>
       </c>
@@ -5354,7 +5610,9 @@
       </c>
     </row>
     <row r="399">
-      <c r="A399" t="inlineStr"/>
+      <c r="A399" t="n">
+        <v>1</v>
+      </c>
       <c r="B399" t="n">
         <v>1.342935149479129e+18</v>
       </c>
@@ -5378,7 +5636,9 @@
       </c>
     </row>
     <row r="401">
-      <c r="A401" t="inlineStr"/>
+      <c r="A401" t="n">
+        <v>1</v>
+      </c>
       <c r="B401" t="n">
         <v>1.342934780518789e+18</v>
       </c>
@@ -5389,7 +5649,9 @@
       </c>
     </row>
     <row r="402">
-      <c r="A402" t="inlineStr"/>
+      <c r="A402" t="n">
+        <v>1</v>
+      </c>
       <c r="B402" t="n">
         <v>1.342934770276303e+18</v>
       </c>
@@ -5569,7 +5831,9 @@
       </c>
     </row>
     <row r="416">
-      <c r="A416" t="inlineStr"/>
+      <c r="A416" t="n">
+        <v>2</v>
+      </c>
       <c r="B416" t="n">
         <v>1.3429323772916e+18</v>
       </c>
@@ -5580,7 +5844,9 @@
       </c>
     </row>
     <row r="417">
-      <c r="A417" t="inlineStr"/>
+      <c r="A417" t="n">
+        <v>2</v>
+      </c>
       <c r="B417" t="n">
         <v>1.342932205174198e+18</v>
       </c>
@@ -5604,7 +5870,9 @@
       </c>
     </row>
     <row r="419">
-      <c r="A419" t="inlineStr"/>
+      <c r="A419" t="n">
+        <v>3</v>
+      </c>
       <c r="B419" t="n">
         <v>1.342932106817786e+18</v>
       </c>
@@ -5615,7 +5883,9 @@
       </c>
     </row>
     <row r="420">
-      <c r="A420" t="inlineStr"/>
+      <c r="A420" t="n">
+        <v>3</v>
+      </c>
       <c r="B420" t="n">
         <v>1.342920919988269e+18</v>
       </c>
@@ -5626,7 +5896,9 @@
       </c>
     </row>
     <row r="421">
-      <c r="A421" t="inlineStr"/>
+      <c r="A421" t="n">
+        <v>1</v>
+      </c>
       <c r="B421" t="n">
         <v>1.342931538737041e+18</v>
       </c>
@@ -5637,7 +5909,9 @@
       </c>
     </row>
     <row r="422">
-      <c r="A422" t="inlineStr"/>
+      <c r="A422" t="n">
+        <v>3</v>
+      </c>
       <c r="B422" t="n">
         <v>1.342931176814567e+18</v>
       </c>
@@ -5648,7 +5922,9 @@
       </c>
     </row>
     <row r="423">
-      <c r="A423" t="inlineStr"/>
+      <c r="A423" t="n">
+        <v>1</v>
+      </c>
       <c r="B423" t="n">
         <v>1.342931048968151e+18</v>
       </c>
@@ -5659,7 +5935,9 @@
       </c>
     </row>
     <row r="424">
-      <c r="A424" t="inlineStr"/>
+      <c r="A424" t="n">
+        <v>1</v>
+      </c>
       <c r="B424" t="n">
         <v>1.34293044618795e+18</v>
       </c>
@@ -5670,7 +5948,9 @@
       </c>
     </row>
     <row r="425">
-      <c r="A425" t="inlineStr"/>
+      <c r="A425" t="n">
+        <v>3</v>
+      </c>
       <c r="B425" t="n">
         <v>1.342930280571613e+18</v>
       </c>
@@ -5681,7 +5961,9 @@
       </c>
     </row>
     <row r="426">
-      <c r="A426" t="inlineStr"/>
+      <c r="A426" t="n">
+        <v>3</v>
+      </c>
       <c r="B426" t="n">
         <v>1.342930149877154e+18</v>
       </c>
@@ -5692,7 +5974,9 @@
       </c>
     </row>
     <row r="427">
-      <c r="A427" t="inlineStr"/>
+      <c r="A427" t="n">
+        <v>1</v>
+      </c>
       <c r="B427" t="n">
         <v>1.342929992267813e+18</v>
       </c>
@@ -5716,7 +6000,9 @@
       </c>
     </row>
     <row r="429">
-      <c r="A429" t="inlineStr"/>
+      <c r="A429" t="n">
+        <v>1</v>
+      </c>
       <c r="B429" t="n">
         <v>1.342929762935837e+18</v>
       </c>
@@ -5727,7 +6013,9 @@
       </c>
     </row>
     <row r="430">
-      <c r="A430" t="inlineStr"/>
+      <c r="A430" t="n">
+        <v>1</v>
+      </c>
       <c r="B430" t="n">
         <v>1.342929594320638e+18</v>
       </c>
@@ -5738,7 +6026,9 @@
       </c>
     </row>
     <row r="431">
-      <c r="A431" t="inlineStr"/>
+      <c r="A431" t="n">
+        <v>2</v>
+      </c>
       <c r="B431" t="n">
         <v>1.342929120334918e+18</v>
       </c>
@@ -5749,7 +6039,9 @@
       </c>
     </row>
     <row r="432">
-      <c r="A432" t="inlineStr"/>
+      <c r="A432" t="n">
+        <v>1</v>
+      </c>
       <c r="B432" t="n">
         <v>1.342928956257874e+18</v>
       </c>
@@ -5760,7 +6052,9 @@
       </c>
     </row>
     <row r="433">
-      <c r="A433" t="inlineStr"/>
+      <c r="A433" t="n">
+        <v>2</v>
+      </c>
       <c r="B433" t="n">
         <v>1.342928930244862e+18</v>
       </c>
@@ -5771,7 +6065,9 @@
       </c>
     </row>
     <row r="434">
-      <c r="A434" t="inlineStr"/>
+      <c r="A434" t="n">
+        <v>1</v>
+      </c>
       <c r="B434" t="n">
         <v>1.342928878386475e+18</v>
       </c>
@@ -5795,7 +6091,9 @@
       </c>
     </row>
     <row r="436">
-      <c r="A436" t="inlineStr"/>
+      <c r="A436" t="n">
+        <v>1</v>
+      </c>
       <c r="B436" t="n">
         <v>1.34292792665276e+18</v>
       </c>
@@ -5806,7 +6104,9 @@
       </c>
     </row>
     <row r="437">
-      <c r="A437" t="inlineStr"/>
+      <c r="A437" t="n">
+        <v>3</v>
+      </c>
       <c r="B437" t="n">
         <v>1.342927561647673e+18</v>
       </c>
@@ -5817,7 +6117,9 @@
       </c>
     </row>
     <row r="438">
-      <c r="A438" t="inlineStr"/>
+      <c r="A438" t="n">
+        <v>1</v>
+      </c>
       <c r="B438" t="n">
         <v>1.342927456563507e+18</v>
       </c>
@@ -5828,7 +6130,9 @@
       </c>
     </row>
     <row r="439">
-      <c r="A439" t="inlineStr"/>
+      <c r="A439" t="n">
+        <v>1</v>
+      </c>
       <c r="B439" t="n">
         <v>1.342927141411951e+18</v>
       </c>
@@ -5839,7 +6143,9 @@
       </c>
     </row>
     <row r="440">
-      <c r="A440" t="inlineStr"/>
+      <c r="A440" t="n">
+        <v>3</v>
+      </c>
       <c r="B440" t="n">
         <v>1.342927007236162e+18</v>
       </c>
@@ -5850,7 +6156,9 @@
       </c>
     </row>
     <row r="441">
-      <c r="A441" t="inlineStr"/>
+      <c r="A441" t="n">
+        <v>1</v>
+      </c>
       <c r="B441" t="n">
         <v>1.342926966320734e+18</v>
       </c>
@@ -5861,7 +6169,9 @@
       </c>
     </row>
     <row r="442">
-      <c r="A442" t="inlineStr"/>
+      <c r="A442" t="n">
+        <v>3</v>
+      </c>
       <c r="B442" t="n">
         <v>1.342926765908488e+18</v>
       </c>
@@ -5872,7 +6182,9 @@
       </c>
     </row>
     <row r="443">
-      <c r="A443" t="inlineStr"/>
+      <c r="A443" t="n">
+        <v>3</v>
+      </c>
       <c r="B443" t="n">
         <v>1.342926713785868e+18</v>
       </c>
@@ -5894,7 +6206,9 @@
       </c>
     </row>
     <row r="445">
-      <c r="A445" t="inlineStr"/>
+      <c r="A445" t="n">
+        <v>1</v>
+      </c>
       <c r="B445" t="n">
         <v>1.332487132846436e+18</v>
       </c>
@@ -5905,7 +6219,9 @@
       </c>
     </row>
     <row r="446">
-      <c r="A446" t="inlineStr"/>
+      <c r="A446" t="n">
+        <v>3</v>
+      </c>
       <c r="B446" t="n">
         <v>1.342926255503639e+18</v>
       </c>
@@ -5916,7 +6232,9 @@
       </c>
     </row>
     <row r="447">
-      <c r="A447" t="inlineStr"/>
+      <c r="A447" t="n">
+        <v>1</v>
+      </c>
       <c r="B447" t="n">
         <v>1.342926181515989e+18</v>
       </c>
@@ -5927,7 +6245,9 @@
       </c>
     </row>
     <row r="448">
-      <c r="A448" t="inlineStr"/>
+      <c r="A448" t="n">
+        <v>2</v>
+      </c>
       <c r="B448" t="n">
         <v>1.342926129334788e+18</v>
       </c>
@@ -5938,7 +6258,9 @@
       </c>
     </row>
     <row r="449">
-      <c r="A449" t="inlineStr"/>
+      <c r="A449" t="n">
+        <v>1</v>
+      </c>
       <c r="B449" t="n">
         <v>1.342926096002671e+18</v>
       </c>
@@ -5949,7 +6271,9 @@
       </c>
     </row>
     <row r="450">
-      <c r="A450" t="inlineStr"/>
+      <c r="A450" t="n">
+        <v>1</v>
+      </c>
       <c r="B450" t="n">
         <v>1.342926023839666e+18</v>
       </c>
@@ -5960,7 +6284,9 @@
       </c>
     </row>
     <row r="451">
-      <c r="A451" t="inlineStr"/>
+      <c r="A451" t="n">
+        <v>2</v>
+      </c>
       <c r="B451" t="n">
         <v>1.342925701339607e+18</v>
       </c>
@@ -5971,7 +6297,9 @@
       </c>
     </row>
     <row r="452">
-      <c r="A452" t="inlineStr"/>
+      <c r="A452" t="n">
+        <v>3</v>
+      </c>
       <c r="B452" t="n">
         <v>1.342925675989242e+18</v>
       </c>
@@ -5995,7 +6323,9 @@
       </c>
     </row>
     <row r="454">
-      <c r="A454" t="inlineStr"/>
+      <c r="A454" t="n">
+        <v>3</v>
+      </c>
       <c r="B454" t="n">
         <v>1.342925331729154e+18</v>
       </c>
@@ -6019,7 +6349,9 @@
       </c>
     </row>
     <row r="456">
-      <c r="A456" t="inlineStr"/>
+      <c r="A456" t="n">
+        <v>1</v>
+      </c>
       <c r="B456" t="n">
         <v>1.3429248613086e+18</v>
       </c>
@@ -6030,7 +6362,9 @@
       </c>
     </row>
     <row r="457">
-      <c r="A457" t="inlineStr"/>
+      <c r="A457" t="n">
+        <v>3</v>
+      </c>
       <c r="B457" t="n">
         <v>1.342924755427586e+18</v>
       </c>
@@ -6041,7 +6375,9 @@
       </c>
     </row>
     <row r="458">
-      <c r="A458" t="inlineStr"/>
+      <c r="A458" t="n">
+        <v>3</v>
+      </c>
       <c r="B458" t="n">
         <v>1.342865922776838e+18</v>
       </c>
@@ -6052,7 +6388,9 @@
       </c>
     </row>
     <row r="459">
-      <c r="A459" t="inlineStr"/>
+      <c r="A459" t="n">
+        <v>3</v>
+      </c>
       <c r="B459" t="n">
         <v>1.342924541341934e+18</v>
       </c>
@@ -6063,7 +6401,9 @@
       </c>
     </row>
     <row r="460">
-      <c r="A460" t="inlineStr"/>
+      <c r="A460" t="n">
+        <v>1</v>
+      </c>
       <c r="B460" t="n">
         <v>1.342924525676204e+18</v>
       </c>
@@ -6074,7 +6414,9 @@
       </c>
     </row>
     <row r="461">
-      <c r="A461" t="inlineStr"/>
+      <c r="A461" t="n">
+        <v>2</v>
+      </c>
       <c r="B461" t="n">
         <v>1.342923962460856e+18</v>
       </c>
@@ -6085,7 +6427,9 @@
       </c>
     </row>
     <row r="462">
-      <c r="A462" t="inlineStr"/>
+      <c r="A462" t="n">
+        <v>1</v>
+      </c>
       <c r="B462" t="n">
         <v>1.34265282354527e+18</v>
       </c>
@@ -6122,7 +6466,9 @@
       </c>
     </row>
     <row r="465">
-      <c r="A465" t="inlineStr"/>
+      <c r="A465" t="n">
+        <v>2</v>
+      </c>
       <c r="B465" t="n">
         <v>1.342922988707e+18</v>
       </c>
@@ -6146,7 +6492,9 @@
       </c>
     </row>
     <row r="467">
-      <c r="A467" t="inlineStr"/>
+      <c r="A467" t="n">
+        <v>2</v>
+      </c>
       <c r="B467" t="n">
         <v>1.342922070922031e+18</v>
       </c>
@@ -6157,7 +6505,9 @@
       </c>
     </row>
     <row r="468">
-      <c r="A468" t="inlineStr"/>
+      <c r="A468" t="n">
+        <v>1</v>
+      </c>
       <c r="B468" t="n">
         <v>1.342922000956875e+18</v>
       </c>
@@ -6181,7 +6531,9 @@
       </c>
     </row>
     <row r="470">
-      <c r="A470" t="inlineStr"/>
+      <c r="A470" t="n">
+        <v>3</v>
+      </c>
       <c r="B470" t="n">
         <v>1.343139148404842e+18</v>
       </c>
@@ -6192,7 +6544,9 @@
       </c>
     </row>
     <row r="471">
-      <c r="A471" t="inlineStr"/>
+      <c r="A471" t="n">
+        <v>1</v>
+      </c>
       <c r="B471" t="n">
         <v>1.342921567257432e+18</v>
       </c>
@@ -6203,7 +6557,9 @@
       </c>
     </row>
     <row r="472">
-      <c r="A472" t="inlineStr"/>
+      <c r="A472" t="n">
+        <v>1</v>
+      </c>
       <c r="B472" t="n">
         <v>1.342921247806644e+18</v>
       </c>
@@ -6214,7 +6570,9 @@
       </c>
     </row>
     <row r="473">
-      <c r="A473" t="inlineStr"/>
+      <c r="A473" t="n">
+        <v>3</v>
+      </c>
       <c r="B473" t="n">
         <v>1.342920940112536e+18</v>
       </c>
@@ -6225,7 +6583,9 @@
       </c>
     </row>
     <row r="474">
-      <c r="A474" t="inlineStr"/>
+      <c r="A474" t="n">
+        <v>1</v>
+      </c>
       <c r="B474" t="n">
         <v>1.342920133073842e+18</v>
       </c>
@@ -6236,7 +6596,9 @@
       </c>
     </row>
     <row r="475">
-      <c r="A475" t="inlineStr"/>
+      <c r="A475" t="n">
+        <v>1</v>
+      </c>
       <c r="B475" t="n">
         <v>1.34310911952443e+18</v>
       </c>
@@ -6247,7 +6609,9 @@
       </c>
     </row>
     <row r="476">
-      <c r="A476" t="inlineStr"/>
+      <c r="A476" t="n">
+        <v>3</v>
+      </c>
       <c r="B476" t="n">
         <v>1.342919936600134e+18</v>
       </c>
@@ -6271,7 +6635,9 @@
       </c>
     </row>
     <row r="478">
-      <c r="A478" t="inlineStr"/>
+      <c r="A478" t="n">
+        <v>3</v>
+      </c>
       <c r="B478" t="n">
         <v>1.342919083701006e+18</v>
       </c>
@@ -6282,7 +6648,9 @@
       </c>
     </row>
     <row r="479">
-      <c r="A479" t="inlineStr"/>
+      <c r="A479" t="n">
+        <v>2</v>
+      </c>
       <c r="B479" t="n">
         <v>1.342918874946273e+18</v>
       </c>
@@ -6293,7 +6661,9 @@
       </c>
     </row>
     <row r="480">
-      <c r="A480" t="inlineStr"/>
+      <c r="A480" t="n">
+        <v>3</v>
+      </c>
       <c r="B480" t="n">
         <v>1.342918655546434e+18</v>
       </c>
@@ -6304,7 +6674,9 @@
       </c>
     </row>
     <row r="481">
-      <c r="A481" t="inlineStr"/>
+      <c r="A481" t="n">
+        <v>3</v>
+      </c>
       <c r="B481" t="n">
         <v>1.342918259117588e+18</v>
       </c>
@@ -6315,7 +6687,9 @@
       </c>
     </row>
     <row r="482">
-      <c r="A482" t="inlineStr"/>
+      <c r="A482" t="n">
+        <v>2</v>
+      </c>
       <c r="B482" t="n">
         <v>1.342918041416438e+18</v>
       </c>
@@ -6326,7 +6700,9 @@
       </c>
     </row>
     <row r="483">
-      <c r="A483" t="inlineStr"/>
+      <c r="A483" t="n">
+        <v>3</v>
+      </c>
       <c r="B483" t="n">
         <v>1.342917923401314e+18</v>
       </c>
@@ -6350,7 +6726,9 @@
       </c>
     </row>
     <row r="485">
-      <c r="A485" t="inlineStr"/>
+      <c r="A485" t="n">
+        <v>3</v>
+      </c>
       <c r="B485" t="n">
         <v>1.34291773749719e+18</v>
       </c>
@@ -6374,7 +6752,9 @@
       </c>
     </row>
     <row r="487">
-      <c r="A487" t="inlineStr"/>
+      <c r="A487" t="n">
+        <v>2</v>
+      </c>
       <c r="B487" t="n">
         <v>1.342917422240702e+18</v>
       </c>
@@ -6385,7 +6765,9 @@
       </c>
     </row>
     <row r="488">
-      <c r="A488" t="inlineStr"/>
+      <c r="A488" t="n">
+        <v>1</v>
+      </c>
       <c r="B488" t="n">
         <v>1.343040664309801e+18</v>
       </c>
@@ -6396,7 +6778,9 @@
       </c>
     </row>
     <row r="489">
-      <c r="A489" t="inlineStr"/>
+      <c r="A489" t="n">
+        <v>1</v>
+      </c>
       <c r="B489" t="n">
         <v>1.342917041121071e+18</v>
       </c>
@@ -6407,7 +6791,9 @@
       </c>
     </row>
     <row r="490">
-      <c r="A490" t="inlineStr"/>
+      <c r="A490" t="n">
+        <v>1</v>
+      </c>
       <c r="B490" t="n">
         <v>1.342916990600684e+18</v>
       </c>
@@ -6431,7 +6817,9 @@
       </c>
     </row>
     <row r="492">
-      <c r="A492" t="inlineStr"/>
+      <c r="A492" t="n">
+        <v>3</v>
+      </c>
       <c r="B492" t="n">
         <v>1.342916807494152e+18</v>
       </c>
@@ -6442,7 +6830,9 @@
       </c>
     </row>
     <row r="493">
-      <c r="A493" t="inlineStr"/>
+      <c r="A493" t="n">
+        <v>2</v>
+      </c>
       <c r="B493" t="n">
         <v>1.342916728402149e+18</v>
       </c>
@@ -6453,7 +6843,9 @@
       </c>
     </row>
     <row r="494">
-      <c r="A494" t="inlineStr"/>
+      <c r="A494" t="n">
+        <v>1</v>
+      </c>
       <c r="B494" t="n">
         <v>1.342916591852388e+18</v>
       </c>
@@ -6464,7 +6856,9 @@
       </c>
     </row>
     <row r="495">
-      <c r="A495" t="inlineStr"/>
+      <c r="A495" t="n">
+        <v>3</v>
+      </c>
       <c r="B495" t="n">
         <v>1.342916489003856e+18</v>
       </c>
@@ -6488,7 +6882,9 @@
       </c>
     </row>
     <row r="497">
-      <c r="A497" t="inlineStr"/>
+      <c r="A497" t="n">
+        <v>3</v>
+      </c>
       <c r="B497" t="n">
         <v>1.342915617117135e+18</v>
       </c>
@@ -6499,7 +6895,9 @@
       </c>
     </row>
     <row r="498">
-      <c r="A498" t="inlineStr"/>
+      <c r="A498" t="n">
+        <v>1</v>
+      </c>
       <c r="B498" t="n">
         <v>1.342915600813847e+18</v>
       </c>
@@ -6510,7 +6908,9 @@
       </c>
     </row>
     <row r="499">
-      <c r="A499" t="inlineStr"/>
+      <c r="A499" t="n">
+        <v>1</v>
+      </c>
       <c r="B499" t="n">
         <v>1.342915544782135e+18</v>
       </c>
@@ -10473,7 +10873,9 @@
       </c>
     </row>
     <row r="804">
-      <c r="A804" t="inlineStr"/>
+      <c r="A804" t="n">
+        <v>3</v>
+      </c>
       <c r="B804" t="n">
         <v>1.342872851624432e+18</v>
       </c>
@@ -10484,7 +10886,9 @@
       </c>
     </row>
     <row r="805">
-      <c r="A805" t="inlineStr"/>
+      <c r="A805" t="n">
+        <v>3</v>
+      </c>
       <c r="B805" t="n">
         <v>1.342872814639067e+18</v>
       </c>
@@ -10495,7 +10899,9 @@
       </c>
     </row>
     <row r="806">
-      <c r="A806" t="inlineStr"/>
+      <c r="A806" t="n">
+        <v>3</v>
+      </c>
       <c r="B806" t="n">
         <v>1.342872490314506e+18</v>
       </c>
@@ -10519,7 +10925,9 @@
       </c>
     </row>
     <row r="808">
-      <c r="A808" t="inlineStr"/>
+      <c r="A808" t="n">
+        <v>3</v>
+      </c>
       <c r="B808" t="n">
         <v>1.342872027133342e+18</v>
       </c>
@@ -10543,7 +10951,9 @@
       </c>
     </row>
     <row r="810">
-      <c r="A810" t="inlineStr"/>
+      <c r="A810" t="n">
+        <v>2</v>
+      </c>
       <c r="B810" t="n">
         <v>1.342871071104532e+18</v>
       </c>
@@ -10554,7 +10964,9 @@
       </c>
     </row>
     <row r="811">
-      <c r="A811" t="inlineStr"/>
+      <c r="A811" t="n">
+        <v>3</v>
+      </c>
       <c r="B811" t="n">
         <v>1.342871050246349e+18</v>
       </c>
@@ -10578,7 +10990,9 @@
       </c>
     </row>
     <row r="813">
-      <c r="A813" t="inlineStr"/>
+      <c r="A813" t="n">
+        <v>3</v>
+      </c>
       <c r="B813" t="n">
         <v>1.34287068988015e+18</v>
       </c>
@@ -10589,7 +11003,9 @@
       </c>
     </row>
     <row r="814">
-      <c r="A814" t="inlineStr"/>
+      <c r="A814" t="n">
+        <v>1</v>
+      </c>
       <c r="B814" t="n">
         <v>1.342870569914683e+18</v>
       </c>
@@ -10600,7 +11016,9 @@
       </c>
     </row>
     <row r="815">
-      <c r="A815" t="inlineStr"/>
+      <c r="A815" t="n">
+        <v>3</v>
+      </c>
       <c r="B815" t="n">
         <v>1.342870364964213e+18</v>
       </c>
@@ -10637,7 +11055,9 @@
       </c>
     </row>
     <row r="818">
-      <c r="A818" t="inlineStr"/>
+      <c r="A818" t="n">
+        <v>2</v>
+      </c>
       <c r="B818" t="n">
         <v>1.342870060029903e+18</v>
       </c>
@@ -10648,7 +11068,9 @@
       </c>
     </row>
     <row r="819">
-      <c r="A819" t="inlineStr"/>
+      <c r="A819" t="n">
+        <v>2</v>
+      </c>
       <c r="B819" t="n">
         <v>1.342870023287808e+18</v>
       </c>
@@ -10659,7 +11081,9 @@
       </c>
     </row>
     <row r="820">
-      <c r="A820" t="inlineStr"/>
+      <c r="A820" t="n">
+        <v>1</v>
+      </c>
       <c r="B820" t="n">
         <v>1.342869958938784e+18</v>
       </c>
@@ -10670,7 +11094,9 @@
       </c>
     </row>
     <row r="821">
-      <c r="A821" t="inlineStr"/>
+      <c r="A821" t="n">
+        <v>2</v>
+      </c>
       <c r="B821" t="n">
         <v>1.342869915741655e+18</v>
       </c>
@@ -10681,7 +11107,9 @@
       </c>
     </row>
     <row r="822">
-      <c r="A822" t="inlineStr"/>
+      <c r="A822" t="n">
+        <v>3</v>
+      </c>
       <c r="B822" t="n">
         <v>1.342869372143067e+18</v>
       </c>
@@ -10692,7 +11120,9 @@
       </c>
     </row>
     <row r="823">
-      <c r="A823" t="inlineStr"/>
+      <c r="A823" t="n">
+        <v>1</v>
+      </c>
       <c r="B823" t="n">
         <v>1.342869365696442e+18</v>
       </c>
@@ -10703,7 +11133,9 @@
       </c>
     </row>
     <row r="824">
-      <c r="A824" t="inlineStr"/>
+      <c r="A824" t="n">
+        <v>3</v>
+      </c>
       <c r="B824" t="n">
         <v>1.342869307856974e+18</v>
       </c>
@@ -10714,7 +11146,9 @@
       </c>
     </row>
     <row r="825">
-      <c r="A825" t="inlineStr"/>
+      <c r="A825" t="n">
+        <v>3</v>
+      </c>
       <c r="B825" t="n">
         <v>1.342869183122571e+18</v>
       </c>
@@ -10725,7 +11159,9 @@
       </c>
     </row>
     <row r="826">
-      <c r="A826" t="inlineStr"/>
+      <c r="A826" t="n">
+        <v>3</v>
+      </c>
       <c r="B826" t="n">
         <v>1.34286904247919e+18</v>
       </c>
@@ -10736,7 +11172,9 @@
       </c>
     </row>
     <row r="827">
-      <c r="A827" t="inlineStr"/>
+      <c r="A827" t="n">
+        <v>1</v>
+      </c>
       <c r="B827" t="n">
         <v>1.342868946467377e+18</v>
       </c>
@@ -10747,7 +11185,9 @@
       </c>
     </row>
     <row r="828">
-      <c r="A828" t="inlineStr"/>
+      <c r="A828" t="n">
+        <v>1</v>
+      </c>
       <c r="B828" t="n">
         <v>1.342868887847772e+18</v>
       </c>
@@ -10758,7 +11198,9 @@
       </c>
     </row>
     <row r="829">
-      <c r="A829" t="inlineStr"/>
+      <c r="A829" t="n">
+        <v>3</v>
+      </c>
       <c r="B829" t="n">
         <v>1.342868702006538e+18</v>
       </c>
@@ -10769,7 +11211,9 @@
       </c>
     </row>
     <row r="830">
-      <c r="A830" t="inlineStr"/>
+      <c r="A830" t="n">
+        <v>3</v>
+      </c>
       <c r="B830" t="n">
         <v>1.342868600374391e+18</v>
       </c>
@@ -10780,7 +11224,9 @@
       </c>
     </row>
     <row r="831">
-      <c r="A831" t="inlineStr"/>
+      <c r="A831" t="n">
+        <v>2</v>
+      </c>
       <c r="B831" t="n">
         <v>1.342868446078513e+18</v>
       </c>
@@ -10791,7 +11237,9 @@
       </c>
     </row>
     <row r="832">
-      <c r="A832" t="inlineStr"/>
+      <c r="A832" t="n">
+        <v>3</v>
+      </c>
       <c r="B832" t="n">
         <v>1.342868411303547e+18</v>
       </c>
@@ -10802,7 +11250,9 @@
       </c>
     </row>
     <row r="833">
-      <c r="A833" t="inlineStr"/>
+      <c r="A833" t="n">
+        <v>3</v>
+      </c>
       <c r="B833" t="n">
         <v>1.342867928191005e+18</v>
       </c>
@@ -10813,7 +11263,9 @@
       </c>
     </row>
     <row r="834">
-      <c r="A834" t="inlineStr"/>
+      <c r="A834" t="n">
+        <v>2</v>
+      </c>
       <c r="B834" t="n">
         <v>1.342867484207149e+18</v>
       </c>
@@ -10824,7 +11276,9 @@
       </c>
     </row>
     <row r="835">
-      <c r="A835" t="inlineStr"/>
+      <c r="A835" t="n">
+        <v>1</v>
+      </c>
       <c r="B835" t="n">
         <v>1.342867083613393e+18</v>
       </c>
@@ -10835,7 +11289,9 @@
       </c>
     </row>
     <row r="836">
-      <c r="A836" t="inlineStr"/>
+      <c r="A836" t="n">
+        <v>3</v>
+      </c>
       <c r="B836" t="n">
         <v>1.342867016848462e+18</v>
       </c>
@@ -10846,7 +11302,9 @@
       </c>
     </row>
     <row r="837">
-      <c r="A837" t="inlineStr"/>
+      <c r="A837" t="n">
+        <v>3</v>
+      </c>
       <c r="B837" t="n">
         <v>1.342867007532884e+18</v>
       </c>
@@ -10857,7 +11315,9 @@
       </c>
     </row>
     <row r="838">
-      <c r="A838" t="inlineStr"/>
+      <c r="A838" t="n">
+        <v>3</v>
+      </c>
       <c r="B838" t="n">
         <v>1.342866933822222e+18</v>
       </c>
@@ -10868,7 +11328,9 @@
       </c>
     </row>
     <row r="839">
-      <c r="A839" t="inlineStr"/>
+      <c r="A839" t="n">
+        <v>3</v>
+      </c>
       <c r="B839" t="n">
         <v>1.342866907750412e+18</v>
       </c>
@@ -10879,7 +11341,9 @@
       </c>
     </row>
     <row r="840">
-      <c r="A840" t="inlineStr"/>
+      <c r="A840" t="n">
+        <v>3</v>
+      </c>
       <c r="B840" t="n">
         <v>1.342866855900414e+18</v>
       </c>
@@ -10890,7 +11354,9 @@
       </c>
     </row>
     <row r="841">
-      <c r="A841" t="inlineStr"/>
+      <c r="A841" t="n">
+        <v>3</v>
+      </c>
       <c r="B841" t="n">
         <v>1.342866722932593e+18</v>
       </c>
@@ -10901,7 +11367,9 @@
       </c>
     </row>
     <row r="842">
-      <c r="A842" t="inlineStr"/>
+      <c r="A842" t="n">
+        <v>3</v>
+      </c>
       <c r="B842" t="n">
         <v>1.342866629919732e+18</v>
       </c>
@@ -10912,7 +11380,9 @@
       </c>
     </row>
     <row r="843">
-      <c r="A843" t="inlineStr"/>
+      <c r="A843" t="n">
+        <v>3</v>
+      </c>
       <c r="B843" t="n">
         <v>1.342866489947398e+18</v>
       </c>
@@ -10923,7 +11393,9 @@
       </c>
     </row>
     <row r="844">
-      <c r="A844" t="inlineStr"/>
+      <c r="A844" t="n">
+        <v>1</v>
+      </c>
       <c r="B844" t="n">
         <v>1.342866106055332e+18</v>
       </c>
@@ -10960,7 +11432,9 @@
       </c>
     </row>
     <row r="847">
-      <c r="A847" t="inlineStr"/>
+      <c r="A847" t="n">
+        <v>3</v>
+      </c>
       <c r="B847" t="n">
         <v>1.342865321108103e+18</v>
       </c>
@@ -10971,7 +11445,9 @@
       </c>
     </row>
     <row r="848">
-      <c r="A848" t="inlineStr"/>
+      <c r="A848" t="n">
+        <v>3</v>
+      </c>
       <c r="B848" t="n">
         <v>1.342865036629463e+18</v>
       </c>
@@ -10982,7 +11458,9 @@
       </c>
     </row>
     <row r="849">
-      <c r="A849" t="inlineStr"/>
+      <c r="A849" t="n">
+        <v>3</v>
+      </c>
       <c r="B849" t="n">
         <v>1.342863109992677e+18</v>
       </c>
@@ -10993,7 +11471,9 @@
       </c>
     </row>
     <row r="850">
-      <c r="A850" t="inlineStr"/>
+      <c r="A850" t="n">
+        <v>3</v>
+      </c>
       <c r="B850" t="n">
         <v>1.342864879678616e+18</v>
       </c>
@@ -11017,7 +11497,9 @@
       </c>
     </row>
     <row r="852">
-      <c r="A852" t="inlineStr"/>
+      <c r="A852" t="n">
+        <v>3</v>
+      </c>
       <c r="B852" t="n">
         <v>1.342864521459855e+18</v>
       </c>
@@ -11028,7 +11510,9 @@
       </c>
     </row>
     <row r="853">
-      <c r="A853" t="inlineStr"/>
+      <c r="A853" t="n">
+        <v>3</v>
+      </c>
       <c r="B853" t="n">
         <v>1.342864072820318e+18</v>
       </c>
@@ -11039,7 +11523,9 @@
       </c>
     </row>
     <row r="854">
-      <c r="A854" t="inlineStr"/>
+      <c r="A854" t="n">
+        <v>3</v>
+      </c>
       <c r="B854" t="n">
         <v>1.342863638785384e+18</v>
       </c>
@@ -11050,7 +11536,9 @@
       </c>
     </row>
     <row r="855">
-      <c r="A855" t="inlineStr"/>
+      <c r="A855" t="n">
+        <v>2</v>
+      </c>
       <c r="B855" t="n">
         <v>1.342863433348354e+18</v>
       </c>
@@ -11061,7 +11549,9 @@
       </c>
     </row>
     <row r="856">
-      <c r="A856" t="inlineStr"/>
+      <c r="A856" t="n">
+        <v>2</v>
+      </c>
       <c r="B856" t="n">
         <v>1.342863295318024e+18</v>
       </c>
@@ -11085,7 +11575,9 @@
       </c>
     </row>
     <row r="858">
-      <c r="A858" t="inlineStr"/>
+      <c r="A858" t="n">
+        <v>3</v>
+      </c>
       <c r="B858" t="n">
         <v>1.342862951762567e+18</v>
       </c>
@@ -11096,7 +11588,9 @@
       </c>
     </row>
     <row r="859">
-      <c r="A859" t="inlineStr"/>
+      <c r="A859" t="n">
+        <v>3</v>
+      </c>
       <c r="B859" t="n">
         <v>1.342862742726693e+18</v>
       </c>
@@ -11107,7 +11601,9 @@
       </c>
     </row>
     <row r="860">
-      <c r="A860" t="inlineStr"/>
+      <c r="A860" t="n">
+        <v>2</v>
+      </c>
       <c r="B860" t="n">
         <v>1.343061901979365e+18</v>
       </c>
@@ -11131,7 +11627,9 @@
       </c>
     </row>
     <row r="862">
-      <c r="A862" t="inlineStr"/>
+      <c r="A862" t="n">
+        <v>3</v>
+      </c>
       <c r="B862" t="n">
         <v>1.342862423963947e+18</v>
       </c>
@@ -11142,7 +11640,9 @@
       </c>
     </row>
     <row r="863">
-      <c r="A863" t="inlineStr"/>
+      <c r="A863" t="n">
+        <v>2</v>
+      </c>
       <c r="B863" t="n">
         <v>1.342759420346982e+18</v>
       </c>
@@ -11153,7 +11653,9 @@
       </c>
     </row>
     <row r="864">
-      <c r="A864" t="inlineStr"/>
+      <c r="A864" t="n">
+        <v>1</v>
+      </c>
       <c r="B864" t="n">
         <v>1.342862306028515e+18</v>
       </c>
@@ -11164,7 +11666,9 @@
       </c>
     </row>
     <row r="865">
-      <c r="A865" t="inlineStr"/>
+      <c r="A865" t="n">
+        <v>1</v>
+      </c>
       <c r="B865" t="n">
         <v>1.342862164126794e+18</v>
       </c>
@@ -11175,7 +11679,9 @@
       </c>
     </row>
     <row r="866">
-      <c r="A866" t="inlineStr"/>
+      <c r="A866" t="n">
+        <v>3</v>
+      </c>
       <c r="B866" t="n">
         <v>1.342862089707278e+18</v>
       </c>
@@ -11186,7 +11692,9 @@
       </c>
     </row>
     <row r="867">
-      <c r="A867" t="inlineStr"/>
+      <c r="A867" t="n">
+        <v>2</v>
+      </c>
       <c r="B867" t="n">
         <v>1.342861825386418e+18</v>
       </c>
@@ -11197,7 +11705,9 @@
       </c>
     </row>
     <row r="868">
-      <c r="A868" t="inlineStr"/>
+      <c r="A868" t="n">
+        <v>1</v>
+      </c>
       <c r="B868" t="n">
         <v>1.342861759175078e+18</v>
       </c>
@@ -11208,7 +11718,9 @@
       </c>
     </row>
     <row r="869">
-      <c r="A869" t="inlineStr"/>
+      <c r="A869" t="n">
+        <v>3</v>
+      </c>
       <c r="B869" t="n">
         <v>1.34286172465603e+18</v>
       </c>
@@ -11219,7 +11731,9 @@
       </c>
     </row>
     <row r="870">
-      <c r="A870" t="inlineStr"/>
+      <c r="A870" t="n">
+        <v>1</v>
+      </c>
       <c r="B870" t="n">
         <v>1.34286169692747e+18</v>
       </c>
@@ -11230,7 +11744,9 @@
       </c>
     </row>
     <row r="871">
-      <c r="A871" t="inlineStr"/>
+      <c r="A871" t="n">
+        <v>3</v>
+      </c>
       <c r="B871" t="n">
         <v>1.342861581009482e+18</v>
       </c>
@@ -11241,7 +11757,9 @@
       </c>
     </row>
     <row r="872">
-      <c r="A872" t="inlineStr"/>
+      <c r="A872" t="n">
+        <v>3</v>
+      </c>
       <c r="B872" t="n">
         <v>1.342861325886755e+18</v>
       </c>
@@ -11252,7 +11770,9 @@
       </c>
     </row>
     <row r="873">
-      <c r="A873" t="inlineStr"/>
+      <c r="A873" t="n">
+        <v>3</v>
+      </c>
       <c r="B873" t="n">
         <v>1.342975958199001e+18</v>
       </c>
@@ -11263,7 +11783,9 @@
       </c>
     </row>
     <row r="874">
-      <c r="A874" t="inlineStr"/>
+      <c r="A874" t="n">
+        <v>3</v>
+      </c>
       <c r="B874" t="n">
         <v>1.342861200556782e+18</v>
       </c>
@@ -11287,7 +11809,9 @@
       </c>
     </row>
     <row r="876">
-      <c r="A876" t="inlineStr"/>
+      <c r="A876" t="n">
+        <v>3</v>
+      </c>
       <c r="B876" t="n">
         <v>1.342860794996863e+18</v>
       </c>
@@ -11298,7 +11822,9 @@
       </c>
     </row>
     <row r="877">
-      <c r="A877" t="inlineStr"/>
+      <c r="A877" t="n">
+        <v>3</v>
+      </c>
       <c r="B877" t="n">
         <v>1.342860760976929e+18</v>
       </c>
@@ -11309,7 +11835,9 @@
       </c>
     </row>
     <row r="878">
-      <c r="A878" t="inlineStr"/>
+      <c r="A878" t="n">
+        <v>3</v>
+      </c>
       <c r="B878" t="n">
         <v>1.342860673345327e+18</v>
       </c>
@@ -11320,7 +11848,9 @@
       </c>
     </row>
     <row r="879">
-      <c r="A879" t="inlineStr"/>
+      <c r="A879" t="n">
+        <v>3</v>
+      </c>
       <c r="B879" t="n">
         <v>1.343235879133966e+18</v>
       </c>
@@ -11331,7 +11861,9 @@
       </c>
     </row>
     <row r="880">
-      <c r="A880" t="inlineStr"/>
+      <c r="A880" t="n">
+        <v>3</v>
+      </c>
       <c r="B880" t="n">
         <v>1.342860074126029e+18</v>
       </c>
@@ -11342,7 +11874,9 @@
       </c>
     </row>
     <row r="881">
-      <c r="A881" t="inlineStr"/>
+      <c r="A881" t="n">
+        <v>1</v>
+      </c>
       <c r="B881" t="n">
         <v>1.342860056518398e+18</v>
       </c>
@@ -11353,7 +11887,9 @@
       </c>
     </row>
     <row r="882">
-      <c r="A882" t="inlineStr"/>
+      <c r="A882" t="n">
+        <v>2</v>
+      </c>
       <c r="B882" t="n">
         <v>1.342859845750428e+18</v>
       </c>
@@ -11364,7 +11900,9 @@
       </c>
     </row>
     <row r="883">
-      <c r="A883" t="inlineStr"/>
+      <c r="A883" t="n">
+        <v>2</v>
+      </c>
       <c r="B883" t="n">
         <v>1.342859796249248e+18</v>
       </c>
@@ -11375,7 +11913,9 @@
       </c>
     </row>
     <row r="884">
-      <c r="A884" t="inlineStr"/>
+      <c r="A884" t="n">
+        <v>1</v>
+      </c>
       <c r="B884" t="n">
         <v>1.342859762057228e+18</v>
       </c>
@@ -11386,7 +11926,9 @@
       </c>
     </row>
     <row r="885">
-      <c r="A885" t="inlineStr"/>
+      <c r="A885" t="n">
+        <v>3</v>
+      </c>
       <c r="B885" t="n">
         <v>1.342859703936811e+18</v>
       </c>
@@ -11397,7 +11939,9 @@
       </c>
     </row>
     <row r="886">
-      <c r="A886" t="inlineStr"/>
+      <c r="A886" t="n">
+        <v>3</v>
+      </c>
       <c r="B886" t="n">
         <v>1.342859546801414e+18</v>
       </c>
@@ -11408,7 +11952,9 @@
       </c>
     </row>
     <row r="887">
-      <c r="A887" t="inlineStr"/>
+      <c r="A887" t="n">
+        <v>2</v>
+      </c>
       <c r="B887" t="n">
         <v>1.342859454006632e+18</v>
       </c>
@@ -11419,7 +11965,9 @@
       </c>
     </row>
     <row r="888">
-      <c r="A888" t="inlineStr"/>
+      <c r="A888" t="n">
+        <v>3</v>
+      </c>
       <c r="B888" t="n">
         <v>1.342859261911642e+18</v>
       </c>
@@ -11430,7 +11978,9 @@
       </c>
     </row>
     <row r="889">
-      <c r="A889" t="inlineStr"/>
+      <c r="A889" t="n">
+        <v>3</v>
+      </c>
       <c r="B889" t="n">
         <v>1.342859133024924e+18</v>
       </c>
@@ -11441,7 +11991,9 @@
       </c>
     </row>
     <row r="890">
-      <c r="A890" t="inlineStr"/>
+      <c r="A890" t="n">
+        <v>3</v>
+      </c>
       <c r="B890" t="n">
         <v>1.342859075227439e+18</v>
       </c>
@@ -11452,7 +12004,9 @@
       </c>
     </row>
     <row r="891">
-      <c r="A891" t="inlineStr"/>
+      <c r="A891" t="n">
+        <v>3</v>
+      </c>
       <c r="B891" t="n">
         <v>1.342859036014883e+18</v>
       </c>
@@ -11463,7 +12017,9 @@
       </c>
     </row>
     <row r="892">
-      <c r="A892" t="inlineStr"/>
+      <c r="A892" t="n">
+        <v>3</v>
+      </c>
       <c r="B892" t="n">
         <v>1.342858666416992e+18</v>
       </c>
@@ -11474,7 +12030,9 @@
       </c>
     </row>
     <row r="893">
-      <c r="A893" t="inlineStr"/>
+      <c r="A893" t="n">
+        <v>3</v>
+      </c>
       <c r="B893" t="n">
         <v>1.3428586610357e+18</v>
       </c>
@@ -11485,7 +12043,9 @@
       </c>
     </row>
     <row r="894">
-      <c r="A894" t="inlineStr"/>
+      <c r="A894" t="n">
+        <v>3</v>
+      </c>
       <c r="B894" t="n">
         <v>1.342858514717434e+18</v>
       </c>
@@ -11509,7 +12069,9 @@
       </c>
     </row>
     <row r="896">
-      <c r="A896" t="inlineStr"/>
+      <c r="A896" t="n">
+        <v>2</v>
+      </c>
       <c r="B896" t="n">
         <v>1.342858278372594e+18</v>
       </c>
@@ -11520,7 +12082,9 @@
       </c>
     </row>
     <row r="897">
-      <c r="A897" t="inlineStr"/>
+      <c r="A897" t="n">
+        <v>3</v>
+      </c>
       <c r="B897" t="n">
         <v>1.342858185263231e+18</v>
       </c>
@@ -11531,7 +12095,9 @@
       </c>
     </row>
     <row r="898">
-      <c r="A898" t="inlineStr"/>
+      <c r="A898" t="n">
+        <v>3</v>
+      </c>
       <c r="B898" t="n">
         <v>1.342857337619571e+18</v>
       </c>
@@ -11555,7 +12121,9 @@
       </c>
     </row>
     <row r="900">
-      <c r="A900" t="inlineStr"/>
+      <c r="A900" t="n">
+        <v>2</v>
+      </c>
       <c r="B900" t="n">
         <v>1.342856680506356e+18</v>
       </c>
@@ -11566,7 +12134,9 @@
       </c>
     </row>
     <row r="901">
-      <c r="A901" t="inlineStr"/>
+      <c r="A901" t="n">
+        <v>3</v>
+      </c>
       <c r="B901" t="n">
         <v>1.342856479880131e+18</v>
       </c>
@@ -11577,7 +12147,9 @@
       </c>
     </row>
     <row r="902">
-      <c r="A902" t="inlineStr"/>
+      <c r="A902" t="n">
+        <v>3</v>
+      </c>
       <c r="B902" t="n">
         <v>1.342856432216117e+18</v>
       </c>
@@ -11588,7 +12160,9 @@
       </c>
     </row>
     <row r="903">
-      <c r="A903" t="inlineStr"/>
+      <c r="A903" t="n">
+        <v>3</v>
+      </c>
       <c r="B903" t="n">
         <v>1.342856410422456e+18</v>
       </c>
@@ -11599,7 +12173,9 @@
       </c>
     </row>
     <row r="904">
-      <c r="A904" t="inlineStr"/>
+      <c r="A904" t="n">
+        <v>2</v>
+      </c>
       <c r="B904" t="n">
         <v>1.342856407868207e+18</v>
       </c>
@@ -11623,7 +12199,9 @@
       </c>
     </row>
     <row r="906">
-      <c r="A906" t="inlineStr"/>
+      <c r="A906" t="n">
+        <v>1</v>
+      </c>
       <c r="B906" t="n">
         <v>1.342856206923215e+18</v>
       </c>
@@ -11647,7 +12225,9 @@
       </c>
     </row>
     <row r="908">
-      <c r="A908" t="inlineStr"/>
+      <c r="A908" t="n">
+        <v>2</v>
+      </c>
       <c r="B908" t="n">
         <v>1.342855748615893e+18</v>
       </c>
@@ -11658,7 +12238,9 @@
       </c>
     </row>
     <row r="909">
-      <c r="A909" t="inlineStr"/>
+      <c r="A909" t="n">
+        <v>3</v>
+      </c>
       <c r="B909" t="n">
         <v>1.342855671025439e+18</v>
       </c>
@@ -11669,7 +12251,9 @@
       </c>
     </row>
     <row r="910">
-      <c r="A910" t="inlineStr"/>
+      <c r="A910" t="n">
+        <v>1</v>
+      </c>
       <c r="B910" t="n">
         <v>1.342855477626106e+18</v>
       </c>
@@ -11680,7 +12264,9 @@
       </c>
     </row>
     <row r="911">
-      <c r="A911" t="inlineStr"/>
+      <c r="A911" t="n">
+        <v>3</v>
+      </c>
       <c r="B911" t="n">
         <v>1.342702242852442e+18</v>
       </c>
@@ -11691,7 +12277,9 @@
       </c>
     </row>
     <row r="912">
-      <c r="A912" t="inlineStr"/>
+      <c r="A912" t="n">
+        <v>3</v>
+      </c>
       <c r="B912" t="n">
         <v>1.342855273770344e+18</v>
       </c>
@@ -11715,7 +12303,9 @@
       </c>
     </row>
     <row r="914">
-      <c r="A914" t="inlineStr"/>
+      <c r="A914" t="n">
+        <v>3</v>
+      </c>
       <c r="B914" t="n">
         <v>1.342855187929723e+18</v>
       </c>
@@ -11726,7 +12316,9 @@
       </c>
     </row>
     <row r="915">
-      <c r="A915" t="inlineStr"/>
+      <c r="A915" t="n">
+        <v>3</v>
+      </c>
       <c r="B915" t="n">
         <v>1.342855048079008e+18</v>
       </c>
@@ -11737,7 +12329,9 @@
       </c>
     </row>
     <row r="916">
-      <c r="A916" t="inlineStr"/>
+      <c r="A916" t="n">
+        <v>1</v>
+      </c>
       <c r="B916" t="n">
         <v>1.329598143994978e+18</v>
       </c>
@@ -11748,7 +12342,9 @@
       </c>
     </row>
     <row r="917">
-      <c r="A917" t="inlineStr"/>
+      <c r="A917" t="n">
+        <v>3</v>
+      </c>
       <c r="B917" t="n">
         <v>1.342854771963793e+18</v>
       </c>
@@ -11772,7 +12368,9 @@
       </c>
     </row>
     <row r="919">
-      <c r="A919" t="inlineStr"/>
+      <c r="A919" t="n">
+        <v>3</v>
+      </c>
       <c r="B919" t="n">
         <v>1.342854644419219e+18</v>
       </c>
@@ -11783,7 +12381,9 @@
       </c>
     </row>
     <row r="920">
-      <c r="A920" t="inlineStr"/>
+      <c r="A920" t="n">
+        <v>3</v>
+      </c>
       <c r="B920" t="n">
         <v>1.342854532817158e+18</v>
       </c>
@@ -11794,7 +12394,9 @@
       </c>
     </row>
     <row r="921">
-      <c r="A921" t="inlineStr"/>
+      <c r="A921" t="n">
+        <v>1</v>
+      </c>
       <c r="B921" t="n">
         <v>1.342854421089288e+18</v>
       </c>
@@ -11805,7 +12407,9 @@
       </c>
     </row>
     <row r="922">
-      <c r="A922" t="inlineStr"/>
+      <c r="A922" t="n">
+        <v>3</v>
+      </c>
       <c r="B922" t="n">
         <v>1.342854328248398e+18</v>
       </c>
@@ -11816,7 +12420,9 @@
       </c>
     </row>
     <row r="923">
-      <c r="A923" t="inlineStr"/>
+      <c r="A923" t="n">
+        <v>3</v>
+      </c>
       <c r="B923" t="n">
         <v>1.342853913993753e+18</v>
       </c>
@@ -11827,7 +12433,9 @@
       </c>
     </row>
     <row r="924">
-      <c r="A924" t="inlineStr"/>
+      <c r="A924" t="n">
+        <v>3</v>
+      </c>
       <c r="B924" t="n">
         <v>1.342853788294668e+18</v>
       </c>
@@ -11838,7 +12446,9 @@
       </c>
     </row>
     <row r="925">
-      <c r="A925" t="inlineStr"/>
+      <c r="A925" t="n">
+        <v>3</v>
+      </c>
       <c r="B925" t="n">
         <v>1.342853709684945e+18</v>
       </c>
@@ -11849,7 +12459,9 @@
       </c>
     </row>
     <row r="926">
-      <c r="A926" t="inlineStr"/>
+      <c r="A926" t="n">
+        <v>2</v>
+      </c>
       <c r="B926" t="n">
         <v>1.342853552927093e+18</v>
       </c>
@@ -11873,7 +12485,9 @@
       </c>
     </row>
     <row r="928">
-      <c r="A928" t="inlineStr"/>
+      <c r="A928" t="n">
+        <v>1</v>
+      </c>
       <c r="B928" t="n">
         <v>1.342852672798527e+18</v>
       </c>
@@ -11884,7 +12498,9 @@
       </c>
     </row>
     <row r="929">
-      <c r="A929" t="inlineStr"/>
+      <c r="A929" t="n">
+        <v>2</v>
+      </c>
       <c r="B929" t="n">
         <v>1.342852619140739e+18</v>
       </c>
@@ -11895,7 +12511,9 @@
       </c>
     </row>
     <row r="930">
-      <c r="A930" t="inlineStr"/>
+      <c r="A930" t="n">
+        <v>3</v>
+      </c>
       <c r="B930" t="n">
         <v>1.342852503310918e+18</v>
       </c>
@@ -11906,7 +12524,9 @@
       </c>
     </row>
     <row r="931">
-      <c r="A931" t="inlineStr"/>
+      <c r="A931" t="n">
+        <v>1</v>
+      </c>
       <c r="B931" t="n">
         <v>1.342852405441024e+18</v>
       </c>
@@ -11917,7 +12537,9 @@
       </c>
     </row>
     <row r="932">
-      <c r="A932" t="inlineStr"/>
+      <c r="A932" t="n">
+        <v>3</v>
+      </c>
       <c r="B932" t="n">
         <v>1.342852386986078e+18</v>
       </c>
@@ -11941,7 +12563,9 @@
       </c>
     </row>
     <row r="934">
-      <c r="A934" t="inlineStr"/>
+      <c r="A934" t="n">
+        <v>3</v>
+      </c>
       <c r="B934" t="n">
         <v>1.342851865264972e+18</v>
       </c>
@@ -11952,7 +12576,9 @@
       </c>
     </row>
     <row r="935">
-      <c r="A935" t="inlineStr"/>
+      <c r="A935" t="n">
+        <v>3</v>
+      </c>
       <c r="B935" t="n">
         <v>1.342851820419494e+18</v>
       </c>
@@ -11963,7 +12589,9 @@
       </c>
     </row>
     <row r="936">
-      <c r="A936" t="inlineStr"/>
+      <c r="A936" t="n">
+        <v>3</v>
+      </c>
       <c r="B936" t="n">
         <v>1.342851344399524e+18</v>
       </c>
@@ -11974,7 +12602,9 @@
       </c>
     </row>
     <row r="937">
-      <c r="A937" t="inlineStr"/>
+      <c r="A937" t="n">
+        <v>1</v>
+      </c>
       <c r="B937" t="n">
         <v>1.343671239907414e+18</v>
       </c>
@@ -11985,7 +12615,9 @@
       </c>
     </row>
     <row r="938">
-      <c r="A938" t="inlineStr"/>
+      <c r="A938" t="n">
+        <v>1</v>
+      </c>
       <c r="B938" t="n">
         <v>1.342851211662393e+18</v>
       </c>
@@ -11996,7 +12628,9 @@
       </c>
     </row>
     <row r="939">
-      <c r="A939" t="inlineStr"/>
+      <c r="A939" t="n">
+        <v>3</v>
+      </c>
       <c r="B939" t="n">
         <v>1.3428499748712e+18</v>
       </c>
@@ -12007,7 +12641,9 @@
       </c>
     </row>
     <row r="940">
-      <c r="A940" t="inlineStr"/>
+      <c r="A940" t="n">
+        <v>3</v>
+      </c>
       <c r="B940" t="n">
         <v>1.34284974815649e+18</v>
       </c>
@@ -12044,7 +12680,9 @@
       </c>
     </row>
     <row r="943">
-      <c r="A943" t="inlineStr"/>
+      <c r="A943" t="n">
+        <v>3</v>
+      </c>
       <c r="B943" t="n">
         <v>1.342849110567739e+18</v>
       </c>
@@ -12055,7 +12693,9 @@
       </c>
     </row>
     <row r="944">
-      <c r="A944" t="inlineStr"/>
+      <c r="A944" t="n">
+        <v>3</v>
+      </c>
       <c r="B944" t="n">
         <v>1.34284891445887e+18</v>
       </c>
@@ -12066,7 +12706,9 @@
       </c>
     </row>
     <row r="945">
-      <c r="A945" t="inlineStr"/>
+      <c r="A945" t="n">
+        <v>3</v>
+      </c>
       <c r="B945" t="n">
         <v>1.34284836089883e+18</v>
       </c>
@@ -12077,7 +12719,9 @@
       </c>
     </row>
     <row r="946">
-      <c r="A946" t="inlineStr"/>
+      <c r="A946" t="n">
+        <v>3</v>
+      </c>
       <c r="B946" t="n">
         <v>1.342848293647364e+18</v>
       </c>
@@ -12088,7 +12732,9 @@
       </c>
     </row>
     <row r="947">
-      <c r="A947" t="inlineStr"/>
+      <c r="A947" t="n">
+        <v>1</v>
+      </c>
       <c r="B947" t="n">
         <v>1.342847129073693e+18</v>
       </c>
@@ -12099,7 +12745,9 @@
       </c>
     </row>
     <row r="948">
-      <c r="A948" t="inlineStr"/>
+      <c r="A948" t="n">
+        <v>1</v>
+      </c>
       <c r="B948" t="n">
         <v>1.342846712516399e+18</v>
       </c>
@@ -12110,7 +12758,9 @@
       </c>
     </row>
     <row r="949">
-      <c r="A949" t="inlineStr"/>
+      <c r="A949" t="n">
+        <v>2</v>
+      </c>
       <c r="B949" t="n">
         <v>1.342846709546807e+18</v>
       </c>
@@ -12121,7 +12771,9 @@
       </c>
     </row>
     <row r="950">
-      <c r="A950" t="inlineStr"/>
+      <c r="A950" t="n">
+        <v>3</v>
+      </c>
       <c r="B950" t="n">
         <v>1.342846697467208e+18</v>
       </c>
@@ -12132,7 +12784,9 @@
       </c>
     </row>
     <row r="951">
-      <c r="A951" t="inlineStr"/>
+      <c r="A951" t="n">
+        <v>3</v>
+      </c>
       <c r="B951" t="n">
         <v>1.343008663498322e+18</v>
       </c>
@@ -12143,7 +12797,9 @@
       </c>
     </row>
     <row r="952">
-      <c r="A952" t="inlineStr"/>
+      <c r="A952" t="n">
+        <v>3</v>
+      </c>
       <c r="B952" t="n">
         <v>1.342846055076008e+18</v>
       </c>
@@ -12154,7 +12810,9 @@
       </c>
     </row>
     <row r="953">
-      <c r="A953" t="inlineStr"/>
+      <c r="A953" t="n">
+        <v>1</v>
+      </c>
       <c r="B953" t="n">
         <v>1.342845958506349e+18</v>
       </c>
@@ -12165,7 +12823,9 @@
       </c>
     </row>
     <row r="954">
-      <c r="A954" t="inlineStr"/>
+      <c r="A954" t="n">
+        <v>3</v>
+      </c>
       <c r="B954" t="n">
         <v>1.34284541734885e+18</v>
       </c>
@@ -12176,7 +12836,9 @@
       </c>
     </row>
     <row r="955">
-      <c r="A955" t="inlineStr"/>
+      <c r="A955" t="n">
+        <v>3</v>
+      </c>
       <c r="B955" t="n">
         <v>1.342845415474024e+18</v>
       </c>
@@ -12187,7 +12849,9 @@
       </c>
     </row>
     <row r="956">
-      <c r="A956" t="inlineStr"/>
+      <c r="A956" t="n">
+        <v>3</v>
+      </c>
       <c r="B956" t="n">
         <v>1.342844903022322e+18</v>
       </c>
@@ -12211,7 +12875,9 @@
       </c>
     </row>
     <row r="958">
-      <c r="A958" t="inlineStr"/>
+      <c r="A958" t="n">
+        <v>3</v>
+      </c>
       <c r="B958" t="n">
         <v>1.342844365396271e+18</v>
       </c>
@@ -12235,7 +12901,9 @@
       </c>
     </row>
     <row r="960">
-      <c r="A960" t="inlineStr"/>
+      <c r="A960" t="n">
+        <v>3</v>
+      </c>
       <c r="B960" t="n">
         <v>1.342844281359376e+18</v>
       </c>
@@ -12246,7 +12914,9 @@
       </c>
     </row>
     <row r="961">
-      <c r="A961" t="inlineStr"/>
+      <c r="A961" t="n">
+        <v>3</v>
+      </c>
       <c r="B961" t="n">
         <v>1.34284363299969e+18</v>
       </c>
@@ -12257,7 +12927,9 @@
       </c>
     </row>
     <row r="962">
-      <c r="A962" t="inlineStr"/>
+      <c r="A962" t="n">
+        <v>2</v>
+      </c>
       <c r="B962" t="n">
         <v>1.342843419450876e+18</v>
       </c>
@@ -12268,7 +12940,9 @@
       </c>
     </row>
     <row r="963">
-      <c r="A963" t="inlineStr"/>
+      <c r="A963" t="n">
+        <v>3</v>
+      </c>
       <c r="B963" t="n">
         <v>1.342843349741535e+18</v>
       </c>
@@ -12279,7 +12953,9 @@
       </c>
     </row>
     <row r="964">
-      <c r="A964" t="inlineStr"/>
+      <c r="A964" t="n">
+        <v>1</v>
+      </c>
       <c r="B964" t="n">
         <v>1.342842952515789e+18</v>
       </c>
@@ -12303,7 +12979,9 @@
       </c>
     </row>
     <row r="966">
-      <c r="A966" t="inlineStr"/>
+      <c r="A966" t="n">
+        <v>1</v>
+      </c>
       <c r="B966" t="n">
         <v>1.342842530744979e+18</v>
       </c>
@@ -12314,7 +12992,9 @@
       </c>
     </row>
     <row r="967">
-      <c r="A967" t="inlineStr"/>
+      <c r="A967" t="n">
+        <v>2</v>
+      </c>
       <c r="B967" t="n">
         <v>1.342842407541465e+18</v>
       </c>
@@ -12325,7 +13005,9 @@
       </c>
     </row>
     <row r="968">
-      <c r="A968" t="inlineStr"/>
+      <c r="A968" t="n">
+        <v>3</v>
+      </c>
       <c r="B968" t="n">
         <v>1.342842114544165e+18</v>
       </c>
@@ -12336,7 +13018,9 @@
       </c>
     </row>
     <row r="969">
-      <c r="A969" t="inlineStr"/>
+      <c r="A969" t="n">
+        <v>3</v>
+      </c>
       <c r="B969" t="n">
         <v>1.342842017278284e+18</v>
       </c>
@@ -12347,7 +13031,9 @@
       </c>
     </row>
     <row r="970">
-      <c r="A970" t="inlineStr"/>
+      <c r="A970" t="n">
+        <v>3</v>
+      </c>
       <c r="B970" t="n">
         <v>1.342841064634388e+18</v>
       </c>
@@ -12358,7 +13044,9 @@
       </c>
     </row>
     <row r="971">
-      <c r="A971" t="inlineStr"/>
+      <c r="A971" t="n">
+        <v>3</v>
+      </c>
       <c r="B971" t="n">
         <v>1.342840950545068e+18</v>
       </c>
@@ -12369,7 +13057,9 @@
       </c>
     </row>
     <row r="972">
-      <c r="A972" t="inlineStr"/>
+      <c r="A972" t="n">
+        <v>1</v>
+      </c>
       <c r="B972" t="n">
         <v>1.342840812321845e+18</v>
       </c>
@@ -12380,7 +13070,9 @@
       </c>
     </row>
     <row r="973">
-      <c r="A973" t="inlineStr"/>
+      <c r="A973" t="n">
+        <v>3</v>
+      </c>
       <c r="B973" t="n">
         <v>1.34284060938043e+18</v>
       </c>
@@ -12391,7 +13083,9 @@
       </c>
     </row>
     <row r="974">
-      <c r="A974" t="inlineStr"/>
+      <c r="A974" t="n">
+        <v>3</v>
+      </c>
       <c r="B974" t="n">
         <v>1.342840475028484e+18</v>
       </c>
@@ -12402,7 +13096,9 @@
       </c>
     </row>
     <row r="975">
-      <c r="A975" t="inlineStr"/>
+      <c r="A975" t="n">
+        <v>3</v>
+      </c>
       <c r="B975" t="n">
         <v>1.342839901163762e+18</v>
       </c>
@@ -12413,7 +13109,9 @@
       </c>
     </row>
     <row r="976">
-      <c r="A976" t="inlineStr"/>
+      <c r="A976" t="n">
+        <v>3</v>
+      </c>
       <c r="B976" t="n">
         <v>1.342839813200884e+18</v>
       </c>
@@ -12424,7 +13122,9 @@
       </c>
     </row>
     <row r="977">
-      <c r="A977" t="inlineStr"/>
+      <c r="A977" t="n">
+        <v>2</v>
+      </c>
       <c r="B977" t="n">
         <v>1.344325167481315e+18</v>
       </c>
@@ -12435,7 +13135,9 @@
       </c>
     </row>
     <row r="978">
-      <c r="A978" t="inlineStr"/>
+      <c r="A978" t="n">
+        <v>3</v>
+      </c>
       <c r="B978" t="n">
         <v>1.344360793157083e+18</v>
       </c>
@@ -12446,7 +13148,9 @@
       </c>
     </row>
     <row r="979">
-      <c r="A979" t="inlineStr"/>
+      <c r="A979" t="n">
+        <v>3</v>
+      </c>
       <c r="B979" t="n">
         <v>1.344324987520487e+18</v>
       </c>
@@ -12457,7 +13161,9 @@
       </c>
     </row>
     <row r="980">
-      <c r="A980" t="inlineStr"/>
+      <c r="A980" t="n">
+        <v>3</v>
+      </c>
       <c r="B980" t="n">
         <v>1.344324826979312e+18</v>
       </c>
@@ -12468,7 +13174,9 @@
       </c>
     </row>
     <row r="981">
-      <c r="A981" t="inlineStr"/>
+      <c r="A981" t="n">
+        <v>3</v>
+      </c>
       <c r="B981" t="n">
         <v>1.344324634066514e+18</v>
       </c>

</xml_diff>